<commit_message>
Implemented conversion to CSS style (issue #1). Renamed source files.
</commit_message>
<xml_diff>
--- a/backend/test/assets/sample.xlsx
+++ b/backend/test/assets/sample.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4507"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Text (with styles)" sheetId="2" r:id="rId1"/>
@@ -13,8 +13,9 @@
     <sheet name="Calculated" sheetId="4" r:id="rId4"/>
     <sheet name="Hidden" sheetId="5" state="hidden" r:id="rId5"/>
     <sheet name="Conditional formatting" sheetId="8" r:id="rId6"/>
+    <sheet name="Colors" sheetId="9" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="125725" iterateDelta="1E-4"/>
+  <calcPr calcId="125725"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="41">
   <si>
     <t>Type</t>
   </si>
@@ -170,9 +171,6 @@
     </r>
   </si>
   <si>
-    <t>Border</t>
-  </si>
-  <si>
     <t>Font</t>
   </si>
   <si>
@@ -243,7 +241,22 @@
     <t>Both</t>
   </si>
   <si>
-    <t>Value</t>
+    <t>Border partial</t>
+  </si>
+  <si>
+    <t>Indent</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>Theme</t>
+  </si>
+  <si>
+    <t>Stanard</t>
   </si>
 </sst>
 </file>
@@ -254,7 +267,7 @@
     <numFmt numFmtId="164" formatCode="[$$-409]#,##0.0;[Red]\-[$$-409]#,##0.0"/>
     <numFmt numFmtId="165" formatCode="#,##0.00\ [$PLN];[Red]\-#,##0.00\ [$PLN]"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -305,8 +318,15 @@
       <color rgb="FF000000"/>
       <name val="Noto Sans"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="25">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -315,24 +335,144 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFF200"/>
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
         <bgColor rgb="FFFFFF00"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="1"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC000"/>
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC00000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0070C0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF7030A0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF002060"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="22">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -357,92 +497,6 @@
     </border>
     <border>
       <left/>
-      <right style="hair">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="hair">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thick">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thick">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thick">
-        <color indexed="64"/>
-      </right>
-      <top style="thick">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thick">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thick">
-        <color indexed="64"/>
-      </top>
-      <bottom style="hair">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
       <right/>
       <top style="hair">
         <color auto="1"/>
@@ -454,15 +508,47 @@
     </border>
     <border>
       <left/>
-      <right style="dotted">
-        <color rgb="FFFF0000"/>
-      </right>
+      <right/>
       <top/>
-      <bottom/>
+      <bottom style="hair">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
-      <left/>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="dotted">
+        <color rgb="FFFF0000"/>
+      </left>
       <right style="dotted">
         <color rgb="FFFF0000"/>
       </right>
@@ -480,98 +566,62 @@
       <top style="dotted">
         <color rgb="FFFF0000"/>
       </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="dashed">
+        <color indexed="64"/>
+      </left>
+      <right style="dashed">
+        <color indexed="64"/>
+      </right>
+      <top style="dashed">
+        <color indexed="64"/>
+      </top>
       <bottom style="dashed">
-        <color theme="3"/>
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="mediumDashed">
+        <color indexed="64"/>
+      </left>
+      <right style="mediumDashed">
+        <color indexed="64"/>
+      </right>
+      <top style="mediumDashed">
+        <color indexed="64"/>
+      </top>
+      <bottom style="mediumDashed">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color indexed="64"/>
+      </left>
+      <right style="double">
+        <color indexed="64"/>
+      </right>
+      <top style="double">
+        <color indexed="64"/>
+      </top>
+      <bottom style="double">
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
-      <right style="dashed">
-        <color theme="3"/>
+      <right style="thin">
+        <color indexed="64"/>
       </right>
       <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="dashed">
-        <color theme="3"/>
-      </right>
-      <top style="dashed">
-        <color theme="3"/>
-      </top>
-      <bottom style="dashed">
-        <color theme="3"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="dashed">
-        <color theme="3"/>
-      </top>
-      <bottom style="double">
-        <color theme="3"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="double">
-        <color theme="3"/>
-      </right>
-      <top style="double">
-        <color theme="3"/>
-      </top>
-      <bottom style="double">
-        <color theme="3"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="double">
-        <color theme="3"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="double">
-        <color theme="3"/>
-      </top>
-      <bottom style="mediumDashed">
-        <color theme="3"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="mediumDashed">
-        <color theme="3"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="mediumDashed">
-        <color theme="3"/>
-      </left>
-      <right style="mediumDashed">
-        <color theme="3"/>
-      </right>
-      <top style="mediumDashed">
-        <color theme="3"/>
-      </top>
-      <bottom style="mediumDashed">
-        <color theme="3"/>
+      <bottom style="thin">
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
@@ -579,7 +629,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -593,42 +643,63 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -702,6 +773,9 @@
       <rgbColor rgb="00333399"/>
       <rgbColor rgb="00333333"/>
     </indexedColors>
+    <mruColors>
+      <color rgb="FFCCECFF"/>
+    </mruColors>
   </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -1003,7 +1077,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1011,10 +1085,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B26"/>
+  <dimension ref="A1:B28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1025,10 +1099,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="7" t="s">
         <v>1</v>
       </c>
     </row>
@@ -1042,153 +1116,163 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B3" s="24" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B5" s="10">
+        <v>5</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" s="8">
         <v>123</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="39.75" customHeight="1">
-      <c r="A6" s="1" t="s">
+    <row r="7" spans="1:2" ht="39.75" customHeight="1">
+      <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B7" s="25" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="37.5" customHeight="1">
-      <c r="A7" s="1" t="s">
+    <row r="8" spans="1:2" ht="37.5" customHeight="1">
+      <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
-      <c r="A8" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="4" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9" t="s">
-        <v>10</v>
+        <v>8</v>
+      </c>
+      <c r="B9" s="26" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B11" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" t="s">
-        <v>15</v>
-      </c>
-      <c r="B12" s="6" t="s">
-        <v>3</v>
+        <v>13</v>
+      </c>
+      <c r="B12" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="20.25">
       <c r="A13" t="s">
-        <v>16</v>
-      </c>
-      <c r="B13" s="13" t="s">
-        <v>30</v>
+        <v>15</v>
+      </c>
+      <c r="B13" s="22" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="14" spans="1:2">
-      <c r="A14" s="15" t="s">
+      <c r="A14" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="B14" s="15"/>
+    </row>
+    <row r="15" spans="1:2" ht="15.75" thickBot="1">
+      <c r="A15" s="10"/>
+      <c r="B15" s="10"/>
+    </row>
+    <row r="16" spans="1:2" ht="16.5" thickTop="1" thickBot="1">
+      <c r="A16" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="B14" s="14"/>
-    </row>
-    <row r="15" spans="1:2" ht="15.75" thickBot="1">
-      <c r="B15" s="16"/>
-    </row>
-    <row r="16" spans="1:2" ht="16.5" thickTop="1" thickBot="1">
-      <c r="A16" s="18" t="s">
+      <c r="B16" s="16"/>
+    </row>
+    <row r="17" spans="1:2" ht="15.75" thickTop="1">
+      <c r="A17" s="10"/>
+      <c r="B17" s="14"/>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="B18" s="11"/>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" s="10"/>
+      <c r="B19" s="12"/>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B20" s="17"/>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" s="9"/>
+      <c r="B21" s="18"/>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="B16" s="17"/>
-    </row>
-    <row r="17" spans="1:2" ht="15.75" thickTop="1">
-      <c r="B17" s="19"/>
-    </row>
-    <row r="18" spans="1:2">
-      <c r="A18" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="B18" s="21"/>
-    </row>
-    <row r="19" spans="1:2">
-      <c r="A19" s="12"/>
-      <c r="B19" s="22"/>
-    </row>
-    <row r="20" spans="1:2">
-      <c r="A20" s="24" t="s">
+      <c r="B22" s="19"/>
+    </row>
+    <row r="23" spans="1:2" ht="15.75" thickBot="1">
+      <c r="A23" s="10"/>
+      <c r="B23" s="10"/>
+    </row>
+    <row r="24" spans="1:2" ht="16.5" thickTop="1" thickBot="1">
+      <c r="A24" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="B20" s="23"/>
-    </row>
-    <row r="21" spans="1:2">
-      <c r="A21" s="11"/>
-      <c r="B21" s="25"/>
-    </row>
-    <row r="22" spans="1:2">
-      <c r="A22" s="27" t="s">
-        <v>25</v>
-      </c>
-      <c r="B22" s="26"/>
-    </row>
-    <row r="23" spans="1:2" ht="15.75" thickBot="1">
-      <c r="B23" s="28"/>
-    </row>
-    <row r="24" spans="1:2" ht="16.5" thickTop="1" thickBot="1">
-      <c r="A24" s="30" t="s">
+      <c r="B24" s="21"/>
+    </row>
+    <row r="25" spans="1:2" ht="16.5" thickTop="1" thickBot="1">
+      <c r="A25" s="10"/>
+      <c r="B25" s="10"/>
+    </row>
+    <row r="26" spans="1:2" ht="15.75" thickBot="1">
+      <c r="A26" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="B24" s="29"/>
-    </row>
-    <row r="25" spans="1:2" ht="16.5" thickTop="1" thickBot="1">
-      <c r="B25" s="31"/>
-    </row>
-    <row r="26" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A26" s="32" t="s">
-        <v>29</v>
-      </c>
-      <c r="B26" s="33"/>
+      <c r="B26" s="20"/>
+    </row>
+    <row r="28" spans="1:2">
+      <c r="A28" t="s">
+        <v>35</v>
+      </c>
+      <c r="B28" s="23"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
@@ -1211,26 +1295,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" s="7" t="s">
         <v>31</v>
-      </c>
-      <c r="B1" s="9" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" t="s">
         <v>33</v>
       </c>
-      <c r="B2" t="s">
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="13" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" s="34" t="s">
-        <v>35</v>
-      </c>
-      <c r="B3" s="34"/>
+      <c r="B3" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1261,7 +1345,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1273,39 +1357,39 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="9" t="s">
-        <v>18</v>
-      </c>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2" s="7">
+      <c r="A2" s="5">
         <v>4</v>
       </c>
-      <c r="B2" s="8">
+      <c r="B2" s="6">
         <f>A2*D$4</f>
         <v>15.16</v>
       </c>
     </row>
     <row r="3" spans="1:4">
-      <c r="A3" s="7">
+      <c r="A3" s="5">
         <v>5</v>
       </c>
-      <c r="B3" s="8">
+      <c r="B3" s="6">
         <f>A3*D$4</f>
         <v>18.95</v>
       </c>
-      <c r="D3" s="9" t="s">
-        <v>19</v>
+      <c r="D3" s="7" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:4">
-      <c r="A4" s="7">
+      <c r="A4" s="5">
         <v>6</v>
       </c>
-      <c r="B4" s="8">
+      <c r="B4" s="6">
         <f>A4*D$4</f>
         <v>22.740000000000002</v>
       </c>
@@ -1314,10 +1398,10 @@
       </c>
     </row>
     <row r="5" spans="1:4">
-      <c r="A5" s="7">
+      <c r="A5" s="5">
         <v>7</v>
       </c>
-      <c r="B5" s="8">
+      <c r="B5" s="6">
         <f>A5*D$4</f>
         <v>26.53</v>
       </c>
@@ -1327,7 +1411,7 @@
         <f>1/0</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="B6" s="8" t="e">
+      <c r="B6" s="6" t="e">
         <f>A6*D$4</f>
         <v>#DIV/0!</v>
       </c>
@@ -1357,10 +1441,10 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" t="s">
         <v>20</v>
-      </c>
-      <c r="B1" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -1383,72 +1467,105 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A11"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:1">
-      <c r="A1" s="9" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1">
+    <row r="1" spans="1:2">
+      <c r="A1" s="31" t="s">
+        <v>37</v>
+      </c>
+      <c r="B1" s="31" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
       <c r="A2">
         <v>10</v>
       </c>
-    </row>
-    <row r="3" spans="1:1">
+      <c r="B2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
       <c r="A3">
         <v>20</v>
       </c>
-    </row>
-    <row r="4" spans="1:1">
+      <c r="B3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
       <c r="A4">
         <v>30</v>
       </c>
-    </row>
-    <row r="5" spans="1:1">
+      <c r="B4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
       <c r="A5">
         <v>40</v>
       </c>
-    </row>
-    <row r="6" spans="1:1">
+      <c r="B5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
       <c r="A6">
         <v>50</v>
       </c>
-    </row>
-    <row r="7" spans="1:1">
+      <c r="B6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
       <c r="A7">
         <v>60</v>
       </c>
-    </row>
-    <row r="8" spans="1:1">
+      <c r="B7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
       <c r="A8">
         <v>70</v>
       </c>
-    </row>
-    <row r="9" spans="1:1">
+      <c r="B8">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
       <c r="A9">
         <v>80</v>
       </c>
-    </row>
-    <row r="10" spans="1:1">
-      <c r="A10">
+      <c r="B9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" s="27">
         <v>90</v>
       </c>
-    </row>
-    <row r="11" spans="1:1">
+      <c r="B10">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
       <c r="A11">
         <v>100</v>
       </c>
+      <c r="B11">
+        <v>10</v>
+      </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:A11">
-    <cfRule type="colorScale" priority="1">
+    <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min" val="0"/>
         <cfvo type="percentile" val="50"/>
@@ -1459,6 +1576,125 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="B2:B11">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF5A8AC6"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="14.28515625" customWidth="1"/>
+    <col min="2" max="2" width="18" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="32" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" s="32" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="33">
+        <v>0</v>
+      </c>
+      <c r="B2" s="40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="30">
+        <v>1</v>
+      </c>
+      <c r="B3" s="41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="29">
+        <v>2</v>
+      </c>
+      <c r="B4" s="42">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="34">
+        <v>3</v>
+      </c>
+      <c r="B5" s="49">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="28">
+        <v>4</v>
+      </c>
+      <c r="B6" s="43">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" s="35">
+        <v>5</v>
+      </c>
+      <c r="B7" s="44">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" s="36">
+        <v>6</v>
+      </c>
+      <c r="B8" s="45">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" s="37">
+        <v>7</v>
+      </c>
+      <c r="B9" s="46">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" s="38">
+        <v>8</v>
+      </c>
+      <c r="B10" s="47">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" s="39">
+        <v>9</v>
+      </c>
+      <c r="B11" s="48">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Implemented color scale handling (issue #5). Adjusted color handling functions. Updated sample XLSX file. Added test target for git retrieval.
</commit_message>
<xml_diff>
--- a/backend/test/assets/sample.xlsx
+++ b/backend/test/assets/sample.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4507"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Text (with styles)" sheetId="2" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="44">
   <si>
     <t>Type</t>
   </si>
@@ -247,16 +247,25 @@
     <t>Indent</t>
   </si>
   <si>
-    <t>A</t>
-  </si>
-  <si>
-    <t>B</t>
-  </si>
-  <si>
     <t>Theme</t>
   </si>
   <si>
     <t>Stanard</t>
+  </si>
+  <si>
+    <t>Number 2</t>
+  </si>
+  <si>
+    <t>Percentile 3</t>
+  </si>
+  <si>
+    <t>Percent 3</t>
+  </si>
+  <si>
+    <t>MinMax 3</t>
+  </si>
+  <si>
+    <t>Formula</t>
   </si>
 </sst>
 </file>
@@ -653,9 +662,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
@@ -700,6 +706,9 @@
     <xf numFmtId="0" fontId="5" fillId="24" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1077,7 +1086,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1118,7 +1127,7 @@
       <c r="A3" t="s">
         <v>36</v>
       </c>
-      <c r="B3" s="24" t="s">
+      <c r="B3" s="23" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1150,7 +1159,7 @@
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="25" t="s">
+      <c r="B7" s="24" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1166,7 +1175,7 @@
       <c r="A9" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="26" t="s">
+      <c r="B9" s="25" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1198,7 +1207,7 @@
       <c r="A13" t="s">
         <v>15</v>
       </c>
-      <c r="B13" s="22" t="s">
+      <c r="B13" s="21" t="s">
         <v>29</v>
       </c>
     </row>
@@ -1206,7 +1215,7 @@
       <c r="A14" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="B14" s="15"/>
+      <c r="B14" s="14"/>
     </row>
     <row r="15" spans="1:2" ht="15.75" thickBot="1">
       <c r="A15" s="10"/>
@@ -1216,11 +1225,11 @@
       <c r="A16" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="B16" s="16"/>
+      <c r="B16" s="15"/>
     </row>
     <row r="17" spans="1:2" ht="15.75" thickTop="1">
       <c r="A17" s="10"/>
-      <c r="B17" s="14"/>
+      <c r="B17" s="13"/>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" s="10" t="s">
@@ -1236,17 +1245,17 @@
       <c r="A20" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="B20" s="17"/>
+      <c r="B20" s="16"/>
     </row>
     <row r="21" spans="1:2">
       <c r="A21" s="9"/>
-      <c r="B21" s="18"/>
+      <c r="B21" s="17"/>
     </row>
     <row r="22" spans="1:2">
       <c r="A22" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="B22" s="19"/>
+      <c r="B22" s="18"/>
     </row>
     <row r="23" spans="1:2" ht="15.75" thickBot="1">
       <c r="A23" s="10"/>
@@ -1256,7 +1265,7 @@
       <c r="A24" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="B24" s="21"/>
+      <c r="B24" s="20"/>
     </row>
     <row r="25" spans="1:2" ht="16.5" thickTop="1" thickBot="1">
       <c r="A25" s="10"/>
@@ -1266,13 +1275,13 @@
       <c r="A26" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="B26" s="20"/>
+      <c r="B26" s="19"/>
     </row>
     <row r="28" spans="1:2">
       <c r="A28" t="s">
         <v>35</v>
       </c>
-      <c r="B28" s="23"/>
+      <c r="B28" s="22"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
@@ -1311,10 +1320,10 @@
       </c>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3" s="13" t="s">
+      <c r="A3" s="49" t="s">
         <v>34</v>
       </c>
-      <c r="B3" s="13"/>
+      <c r="B3" s="49"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1467,105 +1476,211 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="16.7109375" customWidth="1"/>
+    <col min="2" max="2" width="16.5703125" customWidth="1"/>
+    <col min="3" max="3" width="17.28515625" customWidth="1"/>
+    <col min="4" max="4" width="17" customWidth="1"/>
+    <col min="5" max="5" width="20.5703125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" s="31" t="s">
-        <v>37</v>
-      </c>
-      <c r="B1" s="31" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
+    <row r="1" spans="1:5">
+      <c r="A1" s="30" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" s="30" t="s">
+        <v>40</v>
+      </c>
+      <c r="C1" s="30" t="s">
+        <v>41</v>
+      </c>
+      <c r="D1" s="30" t="s">
+        <v>42</v>
+      </c>
+      <c r="E1" s="30" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
       <c r="A2">
         <v>10</v>
       </c>
       <c r="B2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:2">
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
       <c r="A3">
         <v>20</v>
       </c>
       <c r="B3">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:2">
+      <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="D3">
+        <v>2</v>
+      </c>
+      <c r="E3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
       <c r="A4">
         <v>30</v>
       </c>
       <c r="B4">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:2">
+      <c r="C4">
+        <v>3</v>
+      </c>
+      <c r="D4">
+        <v>3</v>
+      </c>
+      <c r="E4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
       <c r="A5">
         <v>40</v>
       </c>
       <c r="B5">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:2">
+      <c r="C5">
+        <v>4</v>
+      </c>
+      <c r="D5">
+        <v>4</v>
+      </c>
+      <c r="E5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
       <c r="A6">
         <v>50</v>
       </c>
       <c r="B6">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:2">
+      <c r="C6">
+        <v>5</v>
+      </c>
+      <c r="D6">
+        <v>5</v>
+      </c>
+      <c r="E6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
       <c r="A7">
         <v>60</v>
       </c>
       <c r="B7">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="1:2">
+      <c r="C7">
+        <v>6</v>
+      </c>
+      <c r="D7">
+        <v>6</v>
+      </c>
+      <c r="E7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
       <c r="A8">
         <v>70</v>
       </c>
       <c r="B8">
         <v>7</v>
       </c>
-    </row>
-    <row r="9" spans="1:2">
+      <c r="C8">
+        <v>7</v>
+      </c>
+      <c r="D8">
+        <v>7</v>
+      </c>
+      <c r="E8">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
       <c r="A9">
         <v>80</v>
       </c>
       <c r="B9">
         <v>8</v>
       </c>
-    </row>
-    <row r="10" spans="1:2">
-      <c r="A10" s="27">
+      <c r="C9">
+        <v>8</v>
+      </c>
+      <c r="D9">
+        <v>8</v>
+      </c>
+      <c r="E9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" s="26">
         <v>90</v>
       </c>
       <c r="B10">
         <v>9</v>
       </c>
-    </row>
-    <row r="11" spans="1:2">
+      <c r="C10">
+        <v>9</v>
+      </c>
+      <c r="D10">
+        <v>9</v>
+      </c>
+      <c r="E10">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
       <c r="A11">
         <v>100</v>
       </c>
       <c r="B11">
         <v>10</v>
       </c>
+      <c r="C11">
+        <v>10</v>
+      </c>
+      <c r="D11">
+        <v>10</v>
+      </c>
+      <c r="E11">
+        <v>10</v>
+      </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:A11">
-    <cfRule type="colorScale" priority="2">
+    <cfRule type="colorScale" priority="6">
       <colorScale>
         <cfvo type="min" val="0"/>
         <cfvo type="percentile" val="50"/>
@@ -1575,12 +1690,44 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
+    <cfRule type="colorScale" priority="4">
+      <colorScale>
+        <cfvo type="num" val="1"/>
+        <cfvo type="num" val="100"/>
+        <color rgb="FFFF7128"/>
+        <color rgb="FFFFEF9C"/>
+      </colorScale>
+    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:B11">
-    <cfRule type="colorScale" priority="1">
+    <cfRule type="colorScale" priority="5">
+      <colorScale>
+        <cfvo type="percentile" val="10"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="percentile" val="90"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF5A8AC6"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C2:C11">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="percent" val="0"/>
+        <cfvo type="percent" val="50"/>
+        <cfvo type="percent" val="100"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF5A8AC6"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D2:D11">
+    <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
+        <cfvo type="percent" val="50"/>
         <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
@@ -1588,7 +1735,20 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="E2:E11">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="formula" val="$C$2+1"/>
+        <cfvo type="formula" val="$D$6"/>
+        <cfvo type="formula" val="$D$10"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF5A8AC6"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967294" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1596,7 +1756,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -1607,90 +1767,90 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="B1" s="32" t="s">
-        <v>40</v>
+      <c r="A1" s="31" t="s">
+        <v>37</v>
+      </c>
+      <c r="B1" s="31" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="33">
+      <c r="A2" s="32">
         <v>0</v>
       </c>
-      <c r="B2" s="40">
+      <c r="B2" s="39">
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3" s="30">
+      <c r="A3" s="29">
         <v>1</v>
       </c>
-      <c r="B3" s="41">
+      <c r="B3" s="40">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:2">
-      <c r="A4" s="29">
+      <c r="A4" s="28">
         <v>2</v>
       </c>
-      <c r="B4" s="42">
+      <c r="B4" s="41">
         <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:2">
-      <c r="A5" s="34">
+      <c r="A5" s="33">
         <v>3</v>
       </c>
-      <c r="B5" s="49">
+      <c r="B5" s="48">
         <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:2">
-      <c r="A6" s="28">
+      <c r="A6" s="27">
         <v>4</v>
       </c>
-      <c r="B6" s="43">
+      <c r="B6" s="42">
         <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:2">
-      <c r="A7" s="35">
+      <c r="A7" s="34">
         <v>5</v>
       </c>
-      <c r="B7" s="44">
+      <c r="B7" s="43">
         <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:2">
-      <c r="A8" s="36">
+      <c r="A8" s="35">
         <v>6</v>
       </c>
-      <c r="B8" s="45">
+      <c r="B8" s="44">
         <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:2">
-      <c r="A9" s="37">
+      <c r="A9" s="36">
         <v>7</v>
       </c>
-      <c r="B9" s="46">
+      <c r="B9" s="45">
         <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:2">
-      <c r="A10" s="38">
+      <c r="A10" s="37">
         <v>8</v>
       </c>
-      <c r="B10" s="47">
+      <c r="B10" s="46">
         <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:2">
-      <c r="A11" s="39">
+      <c r="A11" s="38">
         <v>9</v>
       </c>
-      <c r="B11" s="48">
+      <c r="B11" s="47">
         <v>10</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Keeping empty rows instead of discarding them (issue #1). Omitting hidden rows and columns. Fixed border conversion. Added test cases for styling.
</commit_message>
<xml_diff>
--- a/backend/test/assets/sample.xlsx
+++ b/backend/test/assets/sample.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4507"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Text (with styles)" sheetId="2" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="49">
   <si>
     <t>Type</t>
   </si>
@@ -198,19 +198,58 @@
     <t>Border thick</t>
   </si>
   <si>
-    <t>Border dash</t>
-  </si>
-  <si>
     <t>Border dotted</t>
   </si>
   <si>
-    <t>Border short dash</t>
-  </si>
-  <si>
     <t>Border double</t>
   </si>
   <si>
-    <t>Border thick dash</t>
+    <t>Column A</t>
+  </si>
+  <si>
+    <t>Column B</t>
+  </si>
+  <si>
+    <t>Dog</t>
+  </si>
+  <si>
+    <t>Cat</t>
+  </si>
+  <si>
+    <t>Both</t>
+  </si>
+  <si>
+    <t>Border partial</t>
+  </si>
+  <si>
+    <t>Indent</t>
+  </si>
+  <si>
+    <t>Theme</t>
+  </si>
+  <si>
+    <t>Stanard</t>
+  </si>
+  <si>
+    <t>Number 2</t>
+  </si>
+  <si>
+    <t>Percentile 3</t>
+  </si>
+  <si>
+    <t>Percent 3</t>
+  </si>
+  <si>
+    <t>MinMax 3</t>
+  </si>
+  <si>
+    <t>Formula</t>
+  </si>
+  <si>
+    <t>Align bottom</t>
+  </si>
+  <si>
+    <t>Color</t>
   </si>
   <si>
     <r>
@@ -220,52 +259,29 @@
       <rPr>
         <sz val="16"/>
         <color rgb="FF000000"/>
-        <rFont val="Noto Sans"/>
+        <rFont val="Bauhaus 93"/>
+        <family val="5"/>
       </rPr>
       <t>test</t>
     </r>
   </si>
   <si>
-    <t>Column A</t>
-  </si>
-  <si>
-    <t>Column B</t>
-  </si>
-  <si>
-    <t>Dog</t>
-  </si>
-  <si>
-    <t>Cat</t>
-  </si>
-  <si>
-    <t>Both</t>
-  </si>
-  <si>
-    <t>Border partial</t>
-  </si>
-  <si>
-    <t>Indent</t>
-  </si>
-  <si>
-    <t>Theme</t>
-  </si>
-  <si>
-    <t>Stanard</t>
-  </si>
-  <si>
-    <t>Number 2</t>
-  </si>
-  <si>
-    <t>Percentile 3</t>
-  </si>
-  <si>
-    <t>Percent 3</t>
-  </si>
-  <si>
-    <t>MinMax 3</t>
-  </si>
-  <si>
-    <t>Formula</t>
+    <t>Border thin</t>
+  </si>
+  <si>
+    <t>Border dashed</t>
+  </si>
+  <si>
+    <t>Border thick dashed</t>
+  </si>
+  <si>
+    <t>Hidden</t>
+  </si>
+  <si>
+    <t>Visible</t>
+  </si>
+  <si>
+    <t>Row above is hidden</t>
   </si>
 </sst>
 </file>
@@ -276,7 +292,7 @@
     <numFmt numFmtId="164" formatCode="[$$-409]#,##0.0;[Red]\-[$$-409]#,##0.0"/>
     <numFmt numFmtId="165" formatCode="#,##0.00\ [$PLN];[Red]\-#,##0.00\ [$PLN]"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -310,22 +326,10 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Noto Sans"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="16"/>
-      <color rgb="FF000000"/>
-      <name val="Noto Sans"/>
     </font>
     <font>
       <sz val="11"/>
@@ -333,6 +337,26 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color rgb="FF000000"/>
+      <name val="Bauhaus 93"/>
+      <family val="5"/>
     </font>
   </fonts>
   <fills count="25">
@@ -638,7 +662,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -654,11 +678,10 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -670,13 +693,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -685,10 +704,10 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
@@ -696,19 +715,35 @@
     <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1086,7 +1121,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1094,76 +1129,89 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B28"/>
+  <dimension ref="A1:C33"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="19.5703125" customWidth="1"/>
     <col min="2" max="2" width="33.5703125" customWidth="1"/>
-    <col min="3" max="1025" width="8.5703125" customWidth="1"/>
+    <col min="3" max="3" width="8.5703125" hidden="1" customWidth="1"/>
+    <col min="4" max="1025" width="8.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:3">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="7" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" t="s">
+      <c r="C1" s="7" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="48" t="s">
         <v>2</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" t="s">
-        <v>36</v>
-      </c>
-      <c r="B3" s="23" t="s">
+      <c r="C2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="48" t="s">
+        <v>32</v>
+      </c>
+      <c r="B3" s="21" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" t="s">
+      <c r="C3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="48" t="s">
         <v>4</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5" t="s">
+      <c r="C4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="48" t="s">
         <v>5</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
-      <c r="A6" t="s">
+    <row r="6" spans="1:3">
+      <c r="A6" s="48" t="s">
         <v>21</v>
       </c>
       <c r="B6" s="8">
         <v>123</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="39.75" customHeight="1">
+    <row r="7" spans="1:3" ht="39.75" customHeight="1">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="24" t="s">
+      <c r="B7" s="47" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="37.5" customHeight="1">
+    <row r="8" spans="1:3" ht="37.5" customHeight="1">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
@@ -1171,117 +1219,155 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
-      <c r="A9" t="s">
+    <row r="9" spans="1:3" ht="37.5" customHeight="1">
+      <c r="A9" s="48" t="s">
+        <v>40</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" s="48" t="s">
+        <v>41</v>
+      </c>
+      <c r="B10" s="51" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" s="48" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="25" t="s">
+      <c r="B11" s="22" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
-      <c r="A10" t="s">
+    <row r="12" spans="1:3">
+      <c r="A12" s="48" t="s">
         <v>9</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B12" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
-      <c r="A11" t="s">
+    <row r="13" spans="1:3">
+      <c r="A13" s="48" t="s">
         <v>11</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B13" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
-      <c r="A12" t="s">
+    <row r="14" spans="1:3">
+      <c r="A14" s="48" t="s">
         <v>13</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B14" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="20.25">
-      <c r="A13" t="s">
+    <row r="15" spans="1:3" ht="24.75">
+      <c r="A15" s="48" t="s">
         <v>15</v>
       </c>
-      <c r="B13" s="21" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2">
-      <c r="A14" s="10" t="s">
+      <c r="B15" s="52" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" s="49" t="s">
+        <v>43</v>
+      </c>
+      <c r="B16" s="13"/>
+    </row>
+    <row r="17" spans="1:2" ht="15.75" thickBot="1">
+      <c r="A17" s="49"/>
+      <c r="B17" s="9"/>
+    </row>
+    <row r="18" spans="1:2" ht="16.5" thickTop="1" thickBot="1">
+      <c r="A18" s="49" t="s">
+        <v>23</v>
+      </c>
+      <c r="B18" s="14"/>
+    </row>
+    <row r="19" spans="1:2" ht="15.75" thickTop="1">
+      <c r="A19" s="49"/>
+      <c r="B19" s="12"/>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" s="49" t="s">
         <v>22</v>
       </c>
-      <c r="B14" s="14"/>
-    </row>
-    <row r="15" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A15" s="10"/>
-      <c r="B15" s="10"/>
-    </row>
-    <row r="16" spans="1:2" ht="16.5" thickTop="1" thickBot="1">
-      <c r="A16" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="B16" s="15"/>
-    </row>
-    <row r="17" spans="1:2" ht="15.75" thickTop="1">
-      <c r="A17" s="10"/>
-      <c r="B17" s="13"/>
-    </row>
-    <row r="18" spans="1:2">
-      <c r="A18" s="10" t="s">
+      <c r="B20" s="10"/>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" s="49"/>
+      <c r="B21" s="11"/>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" s="50" t="s">
+        <v>24</v>
+      </c>
+      <c r="B22" s="15"/>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23" s="50"/>
+      <c r="B23" s="16"/>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24" s="50" t="s">
+        <v>44</v>
+      </c>
+      <c r="B24" s="17"/>
+    </row>
+    <row r="25" spans="1:2" ht="15.75" thickBot="1">
+      <c r="A25" s="49"/>
+      <c r="B25" s="9"/>
+    </row>
+    <row r="26" spans="1:2" ht="16.5" thickTop="1" thickBot="1">
+      <c r="A26" s="49" t="s">
         <v>25</v>
       </c>
-      <c r="B18" s="11"/>
-    </row>
-    <row r="19" spans="1:2">
-      <c r="A19" s="10"/>
-      <c r="B19" s="12"/>
-    </row>
-    <row r="20" spans="1:2">
-      <c r="A20" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="B20" s="16"/>
-    </row>
-    <row r="21" spans="1:2">
-      <c r="A21" s="9"/>
-      <c r="B21" s="17"/>
-    </row>
-    <row r="22" spans="1:2">
-      <c r="A22" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="B22" s="18"/>
-    </row>
-    <row r="23" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A23" s="10"/>
-      <c r="B23" s="10"/>
-    </row>
-    <row r="24" spans="1:2" ht="16.5" thickTop="1" thickBot="1">
-      <c r="A24" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="B24" s="20"/>
-    </row>
-    <row r="25" spans="1:2" ht="16.5" thickTop="1" thickBot="1">
-      <c r="A25" s="10"/>
-      <c r="B25" s="10"/>
-    </row>
-    <row r="26" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A26" s="10" t="s">
-        <v>28</v>
-      </c>
       <c r="B26" s="19"/>
     </row>
-    <row r="28" spans="1:2">
-      <c r="A28" t="s">
-        <v>35</v>
-      </c>
-      <c r="B28" s="22"/>
+    <row r="27" spans="1:2" ht="16.5" thickTop="1" thickBot="1">
+      <c r="A27" s="49"/>
+      <c r="B27" s="9"/>
+    </row>
+    <row r="28" spans="1:2" ht="15.75" thickBot="1">
+      <c r="A28" s="49" t="s">
+        <v>45</v>
+      </c>
+      <c r="B28" s="18"/>
+    </row>
+    <row r="29" spans="1:2">
+      <c r="A29" s="48"/>
+    </row>
+    <row r="30" spans="1:2">
+      <c r="A30" s="48" t="s">
+        <v>31</v>
+      </c>
+      <c r="B30" s="20"/>
+    </row>
+    <row r="31" spans="1:2">
+      <c r="A31" s="48"/>
+    </row>
+    <row r="32" spans="1:2" hidden="1">
+      <c r="A32" t="s">
+        <v>46</v>
+      </c>
+      <c r="B32" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2">
+      <c r="A33" s="50" t="s">
+        <v>47</v>
+      </c>
+      <c r="B33" t="s">
+        <v>48</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
@@ -1305,25 +1391,25 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="7" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B2" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3" s="49" t="s">
-        <v>34</v>
-      </c>
-      <c r="B3" s="49"/>
+      <c r="A3" s="46" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3" s="46"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1478,7 +1564,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
@@ -1492,20 +1578,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="27" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1" s="27" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1" s="27" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1" s="27" t="s">
+        <v>38</v>
+      </c>
+      <c r="E1" s="27" t="s">
         <v>39</v>
-      </c>
-      <c r="B1" s="30" t="s">
-        <v>40</v>
-      </c>
-      <c r="C1" s="30" t="s">
-        <v>41</v>
-      </c>
-      <c r="D1" s="30" t="s">
-        <v>42</v>
-      </c>
-      <c r="E1" s="30" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -1645,7 +1731,7 @@
       </c>
     </row>
     <row r="10" spans="1:5">
-      <c r="A10" s="26">
+      <c r="A10" s="23">
         <v>90</v>
       </c>
       <c r="B10">
@@ -1767,90 +1853,90 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" s="31" t="s">
-        <v>37</v>
-      </c>
-      <c r="B1" s="31" t="s">
-        <v>38</v>
+      <c r="A1" s="28" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" s="28" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="32">
+      <c r="A2" s="29">
         <v>0</v>
       </c>
-      <c r="B2" s="39">
+      <c r="B2" s="36">
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3" s="29">
+      <c r="A3" s="26">
         <v>1</v>
       </c>
-      <c r="B3" s="40">
+      <c r="B3" s="37">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:2">
-      <c r="A4" s="28">
+      <c r="A4" s="25">
         <v>2</v>
       </c>
-      <c r="B4" s="41">
+      <c r="B4" s="38">
         <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:2">
-      <c r="A5" s="33">
+      <c r="A5" s="30">
         <v>3</v>
       </c>
-      <c r="B5" s="48">
+      <c r="B5" s="45">
         <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:2">
-      <c r="A6" s="27">
+      <c r="A6" s="24">
         <v>4</v>
       </c>
-      <c r="B6" s="42">
+      <c r="B6" s="39">
         <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:2">
-      <c r="A7" s="34">
+      <c r="A7" s="31">
         <v>5</v>
       </c>
-      <c r="B7" s="43">
+      <c r="B7" s="40">
         <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:2">
-      <c r="A8" s="35">
+      <c r="A8" s="32">
         <v>6</v>
       </c>
-      <c r="B8" s="44">
+      <c r="B8" s="41">
         <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:2">
-      <c r="A9" s="36">
+      <c r="A9" s="33">
         <v>7</v>
       </c>
-      <c r="B9" s="45">
+      <c r="B9" s="42">
         <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:2">
-      <c r="A10" s="37">
+      <c r="A10" s="34">
         <v>8</v>
       </c>
-      <c r="B10" s="46">
+      <c r="B10" s="43">
         <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:2">
-      <c r="A11" s="38">
+      <c r="A11" s="35">
         <v>9</v>
       </c>
-      <c r="B11" s="47">
+      <c r="B11" s="44">
         <v>10</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added unit tests for color scale (issue #5). Fixed time-zone issue. Fixed formatting when cell is in error.
</commit_message>
<xml_diff>
--- a/backend/test/assets/sample.xlsx
+++ b/backend/test/assets/sample.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="50">
   <si>
     <t>Type</t>
   </si>
@@ -283,14 +283,18 @@
   <si>
     <t>Row above is hidden</t>
   </si>
+  <si>
+    <t>Ref</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="[$$-409]#,##0.0;[Red]\-[$$-409]#,##0.0"/>
     <numFmt numFmtId="165" formatCode="#,##0.00\ [$PLN];[Red]\-#,##0.00\ [$PLN]"/>
+    <numFmt numFmtId="166" formatCode="mm/dd/yy;@"/>
   </numFmts>
   <fonts count="9">
     <font>
@@ -662,7 +666,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -700,7 +704,6 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
@@ -725,9 +728,6 @@
     <xf numFmtId="0" fontId="4" fillId="24" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -744,6 +744,18 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1121,7 +1133,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1132,7 +1144,7 @@
   <dimension ref="A1:C33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1155,7 +1167,7 @@
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="48" t="s">
+      <c r="A2" s="46" t="s">
         <v>2</v>
       </c>
       <c r="B2" t="s">
@@ -1166,7 +1178,7 @@
       </c>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" s="48" t="s">
+      <c r="A3" s="46" t="s">
         <v>32</v>
       </c>
       <c r="B3" s="21" t="s">
@@ -1177,7 +1189,7 @@
       </c>
     </row>
     <row r="4" spans="1:3">
-      <c r="A4" s="48" t="s">
+      <c r="A4" s="46" t="s">
         <v>4</v>
       </c>
       <c r="B4" s="2" t="s">
@@ -1188,7 +1200,7 @@
       </c>
     </row>
     <row r="5" spans="1:3">
-      <c r="A5" s="48" t="s">
+      <c r="A5" s="46" t="s">
         <v>5</v>
       </c>
       <c r="B5" s="3" t="s">
@@ -1196,7 +1208,7 @@
       </c>
     </row>
     <row r="6" spans="1:3">
-      <c r="A6" s="48" t="s">
+      <c r="A6" s="46" t="s">
         <v>21</v>
       </c>
       <c r="B6" s="8">
@@ -1207,7 +1219,7 @@
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="47" t="s">
+      <c r="B7" s="45" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1220,7 +1232,7 @@
       </c>
     </row>
     <row r="9" spans="1:3" ht="37.5" customHeight="1">
-      <c r="A9" s="48" t="s">
+      <c r="A9" s="46" t="s">
         <v>40</v>
       </c>
       <c r="B9" s="8" t="s">
@@ -1228,15 +1240,15 @@
       </c>
     </row>
     <row r="10" spans="1:3">
-      <c r="A10" s="48" t="s">
+      <c r="A10" s="46" t="s">
         <v>41</v>
       </c>
-      <c r="B10" s="51" t="s">
+      <c r="B10" s="49" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="11" spans="1:3">
-      <c r="A11" s="48" t="s">
+      <c r="A11" s="46" t="s">
         <v>8</v>
       </c>
       <c r="B11" s="22" t="s">
@@ -1244,7 +1256,7 @@
       </c>
     </row>
     <row r="12" spans="1:3">
-      <c r="A12" s="48" t="s">
+      <c r="A12" s="46" t="s">
         <v>9</v>
       </c>
       <c r="B12" t="s">
@@ -1252,7 +1264,7 @@
       </c>
     </row>
     <row r="13" spans="1:3">
-      <c r="A13" s="48" t="s">
+      <c r="A13" s="46" t="s">
         <v>11</v>
       </c>
       <c r="B13" t="s">
@@ -1260,7 +1272,7 @@
       </c>
     </row>
     <row r="14" spans="1:3">
-      <c r="A14" s="48" t="s">
+      <c r="A14" s="46" t="s">
         <v>13</v>
       </c>
       <c r="B14" t="s">
@@ -1268,90 +1280,90 @@
       </c>
     </row>
     <row r="15" spans="1:3" ht="24.75">
-      <c r="A15" s="48" t="s">
+      <c r="A15" s="46" t="s">
         <v>15</v>
       </c>
-      <c r="B15" s="52" t="s">
+      <c r="B15" s="50" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="16" spans="1:3">
-      <c r="A16" s="49" t="s">
+      <c r="A16" s="47" t="s">
         <v>43</v>
       </c>
       <c r="B16" s="13"/>
     </row>
     <row r="17" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A17" s="49"/>
+      <c r="A17" s="47"/>
       <c r="B17" s="9"/>
     </row>
     <row r="18" spans="1:2" ht="16.5" thickTop="1" thickBot="1">
-      <c r="A18" s="49" t="s">
+      <c r="A18" s="47" t="s">
         <v>23</v>
       </c>
       <c r="B18" s="14"/>
     </row>
     <row r="19" spans="1:2" ht="15.75" thickTop="1">
-      <c r="A19" s="49"/>
+      <c r="A19" s="47"/>
       <c r="B19" s="12"/>
     </row>
     <row r="20" spans="1:2">
-      <c r="A20" s="49" t="s">
+      <c r="A20" s="47" t="s">
         <v>22</v>
       </c>
       <c r="B20" s="10"/>
     </row>
     <row r="21" spans="1:2">
-      <c r="A21" s="49"/>
+      <c r="A21" s="47"/>
       <c r="B21" s="11"/>
     </row>
     <row r="22" spans="1:2">
-      <c r="A22" s="50" t="s">
+      <c r="A22" s="48" t="s">
         <v>24</v>
       </c>
       <c r="B22" s="15"/>
     </row>
     <row r="23" spans="1:2">
-      <c r="A23" s="50"/>
+      <c r="A23" s="48"/>
       <c r="B23" s="16"/>
     </row>
     <row r="24" spans="1:2">
-      <c r="A24" s="50" t="s">
+      <c r="A24" s="48" t="s">
         <v>44</v>
       </c>
       <c r="B24" s="17"/>
     </row>
     <row r="25" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A25" s="49"/>
+      <c r="A25" s="47"/>
       <c r="B25" s="9"/>
     </row>
     <row r="26" spans="1:2" ht="16.5" thickTop="1" thickBot="1">
-      <c r="A26" s="49" t="s">
+      <c r="A26" s="47" t="s">
         <v>25</v>
       </c>
       <c r="B26" s="19"/>
     </row>
     <row r="27" spans="1:2" ht="16.5" thickTop="1" thickBot="1">
-      <c r="A27" s="49"/>
+      <c r="A27" s="47"/>
       <c r="B27" s="9"/>
     </row>
     <row r="28" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A28" s="49" t="s">
+      <c r="A28" s="47" t="s">
         <v>45</v>
       </c>
       <c r="B28" s="18"/>
     </row>
     <row r="29" spans="1:2">
-      <c r="A29" s="48"/>
+      <c r="A29" s="46"/>
     </row>
     <row r="30" spans="1:2">
-      <c r="A30" s="48" t="s">
+      <c r="A30" s="46" t="s">
         <v>31</v>
       </c>
       <c r="B30" s="20"/>
     </row>
     <row r="31" spans="1:2">
-      <c r="A31" s="48"/>
+      <c r="A31" s="46"/>
     </row>
     <row r="32" spans="1:2" hidden="1">
       <c r="A32" t="s">
@@ -1362,7 +1374,7 @@
       </c>
     </row>
     <row r="33" spans="1:2">
-      <c r="A33" s="50" t="s">
+      <c r="A33" s="48" t="s">
         <v>47</v>
       </c>
       <c r="B33" t="s">
@@ -1406,10 +1418,10 @@
       </c>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3" s="46" t="s">
+      <c r="A3" s="54" t="s">
         <v>30</v>
       </c>
-      <c r="B3" s="46"/>
+      <c r="B3" s="54"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1440,7 +1452,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1562,211 +1574,245 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="16.7109375" customWidth="1"/>
-    <col min="2" max="2" width="16.5703125" customWidth="1"/>
-    <col min="3" max="3" width="17.28515625" customWidth="1"/>
-    <col min="4" max="4" width="17" customWidth="1"/>
-    <col min="5" max="5" width="20.5703125" customWidth="1"/>
+    <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
-      <c r="A1" s="27" t="s">
+    <row r="1" spans="1:6">
+      <c r="A1" s="26" t="s">
         <v>35</v>
       </c>
-      <c r="B1" s="27" t="s">
+      <c r="B1" s="26" t="s">
         <v>36</v>
       </c>
-      <c r="C1" s="27" t="s">
+      <c r="C1" s="26" t="s">
         <v>37</v>
       </c>
-      <c r="D1" s="27" t="s">
+      <c r="D1" s="26" t="s">
         <v>38</v>
       </c>
-      <c r="E1" s="27" t="s">
+      <c r="E1" s="26" t="s">
+        <v>49</v>
+      </c>
+      <c r="F1" s="26" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
-      <c r="A2">
+    <row r="2" spans="1:6">
+      <c r="A2" s="51">
         <v>10</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="51">
         <v>1</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="51">
+        <v>-5000</v>
+      </c>
+      <c r="D2" s="53">
+        <v>43831</v>
+      </c>
+      <c r="E2" s="51">
         <v>1</v>
       </c>
-      <c r="D2">
+      <c r="F2" s="51">
         <v>1</v>
       </c>
-      <c r="E2">
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="51">
+        <v>20</v>
+      </c>
+      <c r="B3" s="51">
+        <v>2</v>
+      </c>
+      <c r="C3" s="51">
+        <v>2000</v>
+      </c>
+      <c r="D3" s="53">
+        <v>43832</v>
+      </c>
+      <c r="E3" s="51">
+        <v>2</v>
+      </c>
+      <c r="F3" s="51">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="51">
+        <v>30</v>
+      </c>
+      <c r="B4" s="51">
+        <v>3</v>
+      </c>
+      <c r="C4" s="51">
+        <v>3000</v>
+      </c>
+      <c r="D4" s="53">
+        <v>43833</v>
+      </c>
+      <c r="E4" s="51">
+        <v>3</v>
+      </c>
+      <c r="F4" s="51">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="51">
+        <v>40</v>
+      </c>
+      <c r="B5" s="51">
+        <v>4</v>
+      </c>
+      <c r="C5" s="51">
+        <v>4000</v>
+      </c>
+      <c r="D5" s="53">
+        <v>43834</v>
+      </c>
+      <c r="E5" s="51">
+        <v>4</v>
+      </c>
+      <c r="F5" s="51">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="51">
+        <v>50</v>
+      </c>
+      <c r="B6" s="51">
+        <v>5</v>
+      </c>
+      <c r="C6" s="51">
+        <v>8000</v>
+      </c>
+      <c r="D6" s="53">
+        <v>43835</v>
+      </c>
+      <c r="E6" s="51">
+        <v>5</v>
+      </c>
+      <c r="F6" s="51">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="51">
+        <v>60</v>
+      </c>
+      <c r="B7" s="51">
+        <v>6</v>
+      </c>
+      <c r="C7" s="51">
+        <v>8888</v>
+      </c>
+      <c r="D7" s="53">
+        <v>43836</v>
+      </c>
+      <c r="E7" s="51">
+        <v>6</v>
+      </c>
+      <c r="F7" s="51">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="51">
+        <v>70</v>
+      </c>
+      <c r="B8" s="51">
+        <v>7</v>
+      </c>
+      <c r="C8" s="51">
+        <v>10000</v>
+      </c>
+      <c r="D8" s="53">
+        <v>43837</v>
+      </c>
+      <c r="E8" s="51">
+        <v>7</v>
+      </c>
+      <c r="F8" s="51">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="51">
+        <v>80</v>
+      </c>
+      <c r="B9" s="51">
+        <v>8</v>
+      </c>
+      <c r="C9" s="51">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3">
-        <v>20</v>
-      </c>
-      <c r="B3">
-        <v>2</v>
-      </c>
-      <c r="C3">
-        <v>2</v>
-      </c>
-      <c r="D3">
-        <v>2</v>
-      </c>
-      <c r="E3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4">
-        <v>30</v>
-      </c>
-      <c r="B4">
-        <v>3</v>
-      </c>
-      <c r="C4">
-        <v>3</v>
-      </c>
-      <c r="D4">
-        <v>3</v>
-      </c>
-      <c r="E4">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5">
-        <v>40</v>
-      </c>
-      <c r="B5">
-        <v>4</v>
-      </c>
-      <c r="C5">
-        <v>4</v>
-      </c>
-      <c r="D5">
-        <v>4</v>
-      </c>
-      <c r="E5">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="A6">
-        <v>50</v>
-      </c>
-      <c r="B6">
-        <v>5</v>
-      </c>
-      <c r="C6">
-        <v>5</v>
-      </c>
-      <c r="D6">
-        <v>5</v>
-      </c>
-      <c r="E6">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="A7">
-        <v>60</v>
-      </c>
-      <c r="B7">
-        <v>6</v>
-      </c>
-      <c r="C7">
-        <v>6</v>
-      </c>
-      <c r="D7">
-        <v>6</v>
-      </c>
-      <c r="E7">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
-      <c r="A8">
-        <v>70</v>
-      </c>
-      <c r="B8">
-        <v>7</v>
-      </c>
-      <c r="C8">
-        <v>7</v>
-      </c>
-      <c r="D8">
-        <v>7</v>
-      </c>
-      <c r="E8">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
-      <c r="A9">
-        <v>80</v>
-      </c>
-      <c r="B9">
+      <c r="D9" s="53">
+        <v>43838</v>
+      </c>
+      <c r="E9" s="51">
         <v>8</v>
       </c>
-      <c r="C9">
+      <c r="F9" s="51">
         <v>8</v>
       </c>
-      <c r="D9">
-        <v>8</v>
-      </c>
-      <c r="E9">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5">
-      <c r="A10" s="23">
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" s="52">
         <v>90</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="51">
+        <v>88</v>
+      </c>
+      <c r="C10" s="51">
+        <v>23456</v>
+      </c>
+      <c r="D10" s="53">
+        <v>43839</v>
+      </c>
+      <c r="E10" s="51">
         <v>9</v>
       </c>
-      <c r="C10">
+      <c r="F10" s="51">
         <v>9</v>
       </c>
-      <c r="D10">
-        <v>9</v>
-      </c>
-      <c r="E10">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5">
-      <c r="A11">
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" s="51">
         <v>100</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="51">
+        <v>99</v>
+      </c>
+      <c r="C11" s="51">
+        <v>23</v>
+      </c>
+      <c r="D11" s="53">
+        <v>43840</v>
+      </c>
+      <c r="E11" s="51">
         <v>10</v>
       </c>
-      <c r="C11">
-        <v>10</v>
-      </c>
-      <c r="D11">
-        <v>10</v>
-      </c>
-      <c r="E11">
+      <c r="F11" s="51">
         <v>10</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:A11">
-    <cfRule type="colorScale" priority="6">
+    <cfRule type="colorScale" priority="7">
       <colorScale>
         <cfvo type="min" val="0"/>
         <cfvo type="percentile" val="50"/>
@@ -1776,7 +1822,7 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="colorScale" priority="4">
+    <cfRule type="colorScale" priority="5">
       <colorScale>
         <cfvo type="num" val="1"/>
         <cfvo type="num" val="100"/>
@@ -1786,7 +1832,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:B11">
-    <cfRule type="colorScale" priority="5">
+    <cfRule type="colorScale" priority="6">
       <colorScale>
         <cfvo type="percentile" val="10"/>
         <cfvo type="percentile" val="50"/>
@@ -1798,7 +1844,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2:C11">
-    <cfRule type="colorScale" priority="3">
+    <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="percent" val="0"/>
         <cfvo type="percent" val="50"/>
@@ -1810,7 +1856,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2:D11">
-    <cfRule type="colorScale" priority="2">
+    <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="min" val="0"/>
         <cfvo type="percent" val="50"/>
@@ -1822,11 +1868,23 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:E11">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="formula" val="$B$2"/>
+        <cfvo type="formula" val="$B$6"/>
+        <cfvo type="formula" val="$B$10"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF5A8AC6"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F2:F11">
     <cfRule type="colorScale" priority="1">
       <colorScale>
-        <cfvo type="formula" val="$C$2+1"/>
-        <cfvo type="formula" val="$D$6"/>
-        <cfvo type="formula" val="$D$10"/>
+        <cfvo type="formula" val="$B$2"/>
+        <cfvo type="formula" val="$B$6*4"/>
+        <cfvo type="formula" val="$B$10/2"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF5A8AC6"/>
@@ -1853,90 +1911,90 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="27" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="28" t="s">
+      <c r="B1" s="27" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="29">
+      <c r="A2" s="28">
         <v>0</v>
       </c>
-      <c r="B2" s="36">
+      <c r="B2" s="35">
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3" s="26">
+      <c r="A3" s="25">
         <v>1</v>
       </c>
-      <c r="B3" s="37">
+      <c r="B3" s="36">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:2">
-      <c r="A4" s="25">
+      <c r="A4" s="24">
         <v>2</v>
       </c>
-      <c r="B4" s="38">
+      <c r="B4" s="37">
         <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:2">
-      <c r="A5" s="30">
+      <c r="A5" s="29">
         <v>3</v>
       </c>
-      <c r="B5" s="45">
+      <c r="B5" s="44">
         <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:2">
-      <c r="A6" s="24">
+      <c r="A6" s="23">
         <v>4</v>
       </c>
-      <c r="B6" s="39">
+      <c r="B6" s="38">
         <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:2">
-      <c r="A7" s="31">
+      <c r="A7" s="30">
         <v>5</v>
       </c>
-      <c r="B7" s="40">
+      <c r="B7" s="39">
         <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:2">
-      <c r="A8" s="32">
+      <c r="A8" s="31">
         <v>6</v>
       </c>
-      <c r="B8" s="41">
+      <c r="B8" s="40">
         <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:2">
-      <c r="A9" s="33">
+      <c r="A9" s="32">
         <v>7</v>
       </c>
-      <c r="B9" s="42">
+      <c r="B9" s="41">
         <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:2">
-      <c r="A10" s="34">
+      <c r="A10" s="33">
         <v>8</v>
       </c>
-      <c r="B10" s="43">
+      <c r="B10" s="42">
         <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:2">
-      <c r="A11" s="35">
+      <c r="A11" s="34">
         <v>9</v>
       </c>
-      <c r="B11" s="44">
+      <c r="B11" s="43">
         <v>10</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Handling data bar, icon set, top 10, and above avg. Reworked conditional styling. Refactored style handling slightly.
</commit_message>
<xml_diff>
--- a/backend/test/assets/sample.xlsx
+++ b/backend/test/assets/sample.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4507"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Text (with styles)" sheetId="2" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="84">
   <si>
     <t>Type</t>
   </si>
@@ -286,15 +286,119 @@
   <si>
     <t>Ref</t>
   </si>
+  <si>
+    <t>Data bar 1</t>
+  </si>
+  <si>
+    <t>Data bar 2</t>
+  </si>
+  <si>
+    <t>Top 10%</t>
+  </si>
+  <si>
+    <t>Top 5</t>
+  </si>
+  <si>
+    <t>Bottom 5</t>
+  </si>
+  <si>
+    <t>Above avg</t>
+  </si>
+  <si>
+    <t>Below Avg</t>
+  </si>
+  <si>
+    <t>Icon set 1</t>
+  </si>
+  <si>
+    <t>Icon set 2</t>
+  </si>
+  <si>
+    <t>Icon set 3</t>
+  </si>
+  <si>
+    <t>Greater than</t>
+  </si>
+  <si>
+    <t>Less than</t>
+  </si>
+  <si>
+    <t>Equal</t>
+  </si>
+  <si>
+    <t>Not equal</t>
+  </si>
+  <si>
+    <t>Greater or equal</t>
+  </si>
+  <si>
+    <t>Between</t>
+  </si>
+  <si>
+    <t>Poland</t>
+  </si>
+  <si>
+    <t>Czech Republic</t>
+  </si>
+  <si>
+    <t>Slovakia</t>
+  </si>
+  <si>
+    <t>Hungary</t>
+  </si>
+  <si>
+    <t>Austria</t>
+  </si>
+  <si>
+    <t>Germany</t>
+  </si>
+  <si>
+    <t>Slovenia</t>
+  </si>
+  <si>
+    <t>Finland</t>
+  </si>
+  <si>
+    <t>Switzerland</t>
+  </si>
+  <si>
+    <t>Denmark</t>
+  </si>
+  <si>
+    <t>Contains</t>
+  </si>
+  <si>
+    <t>Ends with</t>
+  </si>
+  <si>
+    <t>Starts with</t>
+  </si>
+  <si>
+    <t>Duplicate</t>
+  </si>
+  <si>
+    <t>Format</t>
+  </si>
+  <si>
+    <t>Unique</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
+  <numFmts count="5">
     <numFmt numFmtId="164" formatCode="[$$-409]#,##0.0;[Red]\-[$$-409]#,##0.0"/>
     <numFmt numFmtId="165" formatCode="#,##0.00\ [$PLN];[Red]\-#,##0.00\ [$PLN]"/>
     <numFmt numFmtId="166" formatCode="mm/dd/yy;@"/>
+    <numFmt numFmtId="168" formatCode="0.00_);[Red]\(0.00\)"/>
+    <numFmt numFmtId="169" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
   <fonts count="9">
     <font>
@@ -666,7 +770,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -753,14 +857,684 @@
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="54">
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFFFF00"/>
+      </font>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFFFF00"/>
+      </font>
+      <numFmt numFmtId="168" formatCode="0.00_);[Red]\(0.00\)"/>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
@@ -1133,7 +1907,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1143,7 +1917,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
@@ -1418,10 +2192,10 @@
       </c>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3" s="54" t="s">
+      <c r="A3" s="57" t="s">
         <v>30</v>
       </c>
-      <c r="B3" s="54"/>
+      <c r="B3" s="57"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1574,10 +2348,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:AC21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView tabSelected="1" topLeftCell="R1" workbookViewId="0">
+      <selection activeCell="AA2" sqref="AA2:AA11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1588,9 +2362,16 @@
     <col min="4" max="4" width="9.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="4" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="23" max="25" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:29">
       <c r="A1" s="26" t="s">
         <v>35</v>
       </c>
@@ -1609,8 +2390,77 @@
       <c r="F1" s="26" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="2" spans="1:6">
+      <c r="G1" s="26" t="s">
+        <v>50</v>
+      </c>
+      <c r="H1" s="26" t="s">
+        <v>51</v>
+      </c>
+      <c r="I1" s="26" t="s">
+        <v>52</v>
+      </c>
+      <c r="J1" s="26" t="s">
+        <v>53</v>
+      </c>
+      <c r="K1" s="26" t="s">
+        <v>54</v>
+      </c>
+      <c r="L1" s="26" t="s">
+        <v>55</v>
+      </c>
+      <c r="M1" s="26" t="s">
+        <v>56</v>
+      </c>
+      <c r="N1" s="26" t="s">
+        <v>57</v>
+      </c>
+      <c r="O1" s="26" t="s">
+        <v>58</v>
+      </c>
+      <c r="P1" s="26" t="s">
+        <v>59</v>
+      </c>
+      <c r="Q1" s="26" t="s">
+        <v>60</v>
+      </c>
+      <c r="R1" s="26" t="s">
+        <v>61</v>
+      </c>
+      <c r="S1" s="26" t="s">
+        <v>62</v>
+      </c>
+      <c r="T1" s="26" t="s">
+        <v>63</v>
+      </c>
+      <c r="U1" s="26" t="s">
+        <v>64</v>
+      </c>
+      <c r="V1" s="26" t="s">
+        <v>65</v>
+      </c>
+      <c r="W1" s="26" t="s">
+        <v>76</v>
+      </c>
+      <c r="X1" s="26" t="s">
+        <v>77</v>
+      </c>
+      <c r="Y1" s="26" t="s">
+        <v>78</v>
+      </c>
+      <c r="Z1" s="26" t="s">
+        <v>79</v>
+      </c>
+      <c r="AA1" s="26" t="s">
+        <v>80</v>
+      </c>
+      <c r="AB1" s="26" t="s">
+        <v>81</v>
+      </c>
+      <c r="AC1" s="26" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="2" spans="1:29">
       <c r="A2" s="51">
         <v>10</v>
       </c>
@@ -1629,8 +2479,77 @@
       <c r="F2" s="51">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:6">
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <v>1</v>
+      </c>
+      <c r="I2">
+        <v>1</v>
+      </c>
+      <c r="J2">
+        <v>10</v>
+      </c>
+      <c r="K2">
+        <v>10</v>
+      </c>
+      <c r="L2">
+        <v>10</v>
+      </c>
+      <c r="M2" s="58">
+        <v>-10</v>
+      </c>
+      <c r="N2">
+        <v>1</v>
+      </c>
+      <c r="O2">
+        <v>1</v>
+      </c>
+      <c r="P2">
+        <v>1</v>
+      </c>
+      <c r="Q2">
+        <v>1</v>
+      </c>
+      <c r="R2">
+        <v>1</v>
+      </c>
+      <c r="S2">
+        <v>1</v>
+      </c>
+      <c r="T2">
+        <v>1</v>
+      </c>
+      <c r="U2">
+        <v>1</v>
+      </c>
+      <c r="V2">
+        <v>1</v>
+      </c>
+      <c r="W2" t="s">
+        <v>66</v>
+      </c>
+      <c r="X2" t="s">
+        <v>66</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>66</v>
+      </c>
+      <c r="Z2">
+        <v>1</v>
+      </c>
+      <c r="AA2" s="59">
+        <v>1</v>
+      </c>
+      <c r="AB2">
+        <v>10</v>
+      </c>
+      <c r="AC2" s="56">
+        <v>44136</v>
+      </c>
+    </row>
+    <row r="3" spans="1:29">
       <c r="A3" s="51">
         <v>20</v>
       </c>
@@ -1649,8 +2568,77 @@
       <c r="F3" s="51">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:6">
+      <c r="G3">
+        <v>2</v>
+      </c>
+      <c r="H3">
+        <v>2</v>
+      </c>
+      <c r="I3">
+        <v>2</v>
+      </c>
+      <c r="J3">
+        <v>20</v>
+      </c>
+      <c r="K3">
+        <v>20</v>
+      </c>
+      <c r="L3">
+        <v>20</v>
+      </c>
+      <c r="M3" s="58">
+        <v>20</v>
+      </c>
+      <c r="N3">
+        <v>2</v>
+      </c>
+      <c r="O3">
+        <v>2</v>
+      </c>
+      <c r="P3">
+        <v>2</v>
+      </c>
+      <c r="Q3">
+        <v>2</v>
+      </c>
+      <c r="R3">
+        <v>2</v>
+      </c>
+      <c r="S3">
+        <v>2</v>
+      </c>
+      <c r="T3">
+        <v>2</v>
+      </c>
+      <c r="U3">
+        <v>2</v>
+      </c>
+      <c r="V3">
+        <v>2</v>
+      </c>
+      <c r="W3" t="s">
+        <v>67</v>
+      </c>
+      <c r="X3" t="s">
+        <v>67</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>67</v>
+      </c>
+      <c r="Z3">
+        <v>2</v>
+      </c>
+      <c r="AA3" s="59">
+        <v>2</v>
+      </c>
+      <c r="AB3">
+        <v>10</v>
+      </c>
+      <c r="AC3" s="56">
+        <v>44137</v>
+      </c>
+    </row>
+    <row r="4" spans="1:29">
       <c r="A4" s="51">
         <v>30</v>
       </c>
@@ -1669,8 +2657,77 @@
       <c r="F4" s="51">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:6">
+      <c r="G4">
+        <v>3</v>
+      </c>
+      <c r="H4">
+        <v>3</v>
+      </c>
+      <c r="I4">
+        <v>3</v>
+      </c>
+      <c r="J4">
+        <v>30</v>
+      </c>
+      <c r="K4">
+        <v>30</v>
+      </c>
+      <c r="L4">
+        <v>30</v>
+      </c>
+      <c r="M4" s="58">
+        <v>30</v>
+      </c>
+      <c r="N4">
+        <v>3</v>
+      </c>
+      <c r="O4">
+        <v>3</v>
+      </c>
+      <c r="P4">
+        <v>3</v>
+      </c>
+      <c r="Q4">
+        <v>3</v>
+      </c>
+      <c r="R4">
+        <v>3</v>
+      </c>
+      <c r="S4">
+        <v>3</v>
+      </c>
+      <c r="T4">
+        <v>3</v>
+      </c>
+      <c r="U4">
+        <v>3</v>
+      </c>
+      <c r="V4">
+        <v>3</v>
+      </c>
+      <c r="W4" t="s">
+        <v>68</v>
+      </c>
+      <c r="X4" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y4" t="s">
+        <v>68</v>
+      </c>
+      <c r="Z4">
+        <v>3</v>
+      </c>
+      <c r="AA4" s="59">
+        <v>-3</v>
+      </c>
+      <c r="AB4">
+        <v>11</v>
+      </c>
+      <c r="AC4" s="56">
+        <v>44138</v>
+      </c>
+    </row>
+    <row r="5" spans="1:29">
       <c r="A5" s="51">
         <v>40</v>
       </c>
@@ -1689,8 +2746,77 @@
       <c r="F5" s="51">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:6">
+      <c r="G5">
+        <v>4</v>
+      </c>
+      <c r="H5">
+        <v>4</v>
+      </c>
+      <c r="I5">
+        <v>4</v>
+      </c>
+      <c r="J5">
+        <v>40</v>
+      </c>
+      <c r="K5">
+        <v>40</v>
+      </c>
+      <c r="L5">
+        <v>40</v>
+      </c>
+      <c r="M5" s="58">
+        <v>40</v>
+      </c>
+      <c r="N5">
+        <v>4</v>
+      </c>
+      <c r="O5">
+        <v>4</v>
+      </c>
+      <c r="P5">
+        <v>4</v>
+      </c>
+      <c r="Q5">
+        <v>4</v>
+      </c>
+      <c r="R5">
+        <v>4</v>
+      </c>
+      <c r="S5">
+        <v>4</v>
+      </c>
+      <c r="T5">
+        <v>4</v>
+      </c>
+      <c r="U5">
+        <v>4</v>
+      </c>
+      <c r="V5">
+        <v>4</v>
+      </c>
+      <c r="W5" t="s">
+        <v>69</v>
+      </c>
+      <c r="X5" t="s">
+        <v>69</v>
+      </c>
+      <c r="Y5" t="s">
+        <v>69</v>
+      </c>
+      <c r="Z5">
+        <v>4</v>
+      </c>
+      <c r="AA5" s="59">
+        <v>-4</v>
+      </c>
+      <c r="AB5">
+        <v>10</v>
+      </c>
+      <c r="AC5" s="56">
+        <v>44139</v>
+      </c>
+    </row>
+    <row r="6" spans="1:29">
       <c r="A6" s="51">
         <v>50</v>
       </c>
@@ -1709,8 +2835,77 @@
       <c r="F6" s="51">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:6">
+      <c r="G6">
+        <v>5</v>
+      </c>
+      <c r="H6">
+        <v>5</v>
+      </c>
+      <c r="I6">
+        <v>5</v>
+      </c>
+      <c r="J6">
+        <v>50</v>
+      </c>
+      <c r="K6">
+        <v>50</v>
+      </c>
+      <c r="L6">
+        <v>50</v>
+      </c>
+      <c r="M6" s="58">
+        <v>50</v>
+      </c>
+      <c r="N6">
+        <v>5</v>
+      </c>
+      <c r="O6">
+        <v>5</v>
+      </c>
+      <c r="P6">
+        <v>5</v>
+      </c>
+      <c r="Q6">
+        <v>5</v>
+      </c>
+      <c r="R6">
+        <v>5</v>
+      </c>
+      <c r="S6">
+        <v>5</v>
+      </c>
+      <c r="T6">
+        <v>5</v>
+      </c>
+      <c r="U6">
+        <v>5</v>
+      </c>
+      <c r="V6">
+        <v>5</v>
+      </c>
+      <c r="W6" t="s">
+        <v>70</v>
+      </c>
+      <c r="X6" t="s">
+        <v>70</v>
+      </c>
+      <c r="Y6" t="s">
+        <v>70</v>
+      </c>
+      <c r="Z6">
+        <v>10</v>
+      </c>
+      <c r="AA6" s="59">
+        <v>-5</v>
+      </c>
+      <c r="AB6">
+        <v>10</v>
+      </c>
+      <c r="AC6" s="56">
+        <v>44140</v>
+      </c>
+    </row>
+    <row r="7" spans="1:29">
       <c r="A7" s="51">
         <v>60</v>
       </c>
@@ -1729,8 +2924,77 @@
       <c r="F7" s="51">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="1:6">
+      <c r="G7">
+        <v>6</v>
+      </c>
+      <c r="H7" s="54">
+        <v>6</v>
+      </c>
+      <c r="I7">
+        <v>6</v>
+      </c>
+      <c r="J7">
+        <v>60</v>
+      </c>
+      <c r="K7">
+        <v>60</v>
+      </c>
+      <c r="L7">
+        <v>60</v>
+      </c>
+      <c r="M7" s="58">
+        <v>60</v>
+      </c>
+      <c r="N7">
+        <v>6</v>
+      </c>
+      <c r="O7">
+        <v>6</v>
+      </c>
+      <c r="P7">
+        <v>6</v>
+      </c>
+      <c r="Q7">
+        <v>6</v>
+      </c>
+      <c r="R7">
+        <v>6</v>
+      </c>
+      <c r="S7">
+        <v>6</v>
+      </c>
+      <c r="T7">
+        <v>6</v>
+      </c>
+      <c r="U7">
+        <v>6</v>
+      </c>
+      <c r="V7">
+        <v>6</v>
+      </c>
+      <c r="W7" t="s">
+        <v>71</v>
+      </c>
+      <c r="X7" t="s">
+        <v>71</v>
+      </c>
+      <c r="Y7" t="s">
+        <v>71</v>
+      </c>
+      <c r="Z7">
+        <v>6</v>
+      </c>
+      <c r="AA7" s="59">
+        <v>6</v>
+      </c>
+      <c r="AB7">
+        <v>20</v>
+      </c>
+      <c r="AC7" s="56">
+        <v>44141</v>
+      </c>
+    </row>
+    <row r="8" spans="1:29">
       <c r="A8" s="51">
         <v>70</v>
       </c>
@@ -1749,8 +3013,77 @@
       <c r="F8" s="51">
         <v>7</v>
       </c>
-    </row>
-    <row r="9" spans="1:6">
+      <c r="G8">
+        <v>7</v>
+      </c>
+      <c r="H8">
+        <v>7</v>
+      </c>
+      <c r="I8">
+        <v>7</v>
+      </c>
+      <c r="J8">
+        <v>70</v>
+      </c>
+      <c r="K8">
+        <v>70</v>
+      </c>
+      <c r="L8">
+        <v>70</v>
+      </c>
+      <c r="M8" s="58">
+        <v>70</v>
+      </c>
+      <c r="N8">
+        <v>7</v>
+      </c>
+      <c r="O8">
+        <v>7</v>
+      </c>
+      <c r="P8">
+        <v>7</v>
+      </c>
+      <c r="Q8">
+        <v>7</v>
+      </c>
+      <c r="R8">
+        <v>7</v>
+      </c>
+      <c r="S8">
+        <v>7</v>
+      </c>
+      <c r="T8">
+        <v>7</v>
+      </c>
+      <c r="U8">
+        <v>7</v>
+      </c>
+      <c r="V8">
+        <v>7</v>
+      </c>
+      <c r="W8" t="s">
+        <v>72</v>
+      </c>
+      <c r="X8" t="s">
+        <v>72</v>
+      </c>
+      <c r="Y8" t="s">
+        <v>72</v>
+      </c>
+      <c r="Z8">
+        <v>7</v>
+      </c>
+      <c r="AA8" s="59">
+        <v>7</v>
+      </c>
+      <c r="AB8">
+        <v>20</v>
+      </c>
+      <c r="AC8" s="56">
+        <v>44142</v>
+      </c>
+    </row>
+    <row r="9" spans="1:29">
       <c r="A9" s="51">
         <v>80</v>
       </c>
@@ -1769,8 +3102,77 @@
       <c r="F9" s="51">
         <v>8</v>
       </c>
-    </row>
-    <row r="10" spans="1:6">
+      <c r="G9">
+        <v>8</v>
+      </c>
+      <c r="H9">
+        <v>8</v>
+      </c>
+      <c r="I9">
+        <v>8</v>
+      </c>
+      <c r="J9">
+        <v>80</v>
+      </c>
+      <c r="K9">
+        <v>80</v>
+      </c>
+      <c r="L9">
+        <v>80</v>
+      </c>
+      <c r="M9" s="58">
+        <v>80</v>
+      </c>
+      <c r="N9">
+        <v>8</v>
+      </c>
+      <c r="O9">
+        <v>8</v>
+      </c>
+      <c r="P9">
+        <v>8</v>
+      </c>
+      <c r="Q9">
+        <v>8</v>
+      </c>
+      <c r="R9">
+        <v>8</v>
+      </c>
+      <c r="S9">
+        <v>8</v>
+      </c>
+      <c r="T9">
+        <v>8</v>
+      </c>
+      <c r="U9">
+        <v>8</v>
+      </c>
+      <c r="V9">
+        <v>8</v>
+      </c>
+      <c r="W9" t="s">
+        <v>73</v>
+      </c>
+      <c r="X9" t="s">
+        <v>73</v>
+      </c>
+      <c r="Y9" t="s">
+        <v>73</v>
+      </c>
+      <c r="Z9">
+        <v>10</v>
+      </c>
+      <c r="AA9" s="59">
+        <v>8</v>
+      </c>
+      <c r="AB9">
+        <v>10</v>
+      </c>
+      <c r="AC9" s="56">
+        <v>44143</v>
+      </c>
+    </row>
+    <row r="10" spans="1:29">
       <c r="A10" s="52">
         <v>90</v>
       </c>
@@ -1789,8 +3191,77 @@
       <c r="F10" s="51">
         <v>9</v>
       </c>
-    </row>
-    <row r="11" spans="1:6">
+      <c r="G10">
+        <v>9</v>
+      </c>
+      <c r="H10">
+        <v>9</v>
+      </c>
+      <c r="I10">
+        <v>9</v>
+      </c>
+      <c r="J10">
+        <v>90</v>
+      </c>
+      <c r="K10">
+        <v>90</v>
+      </c>
+      <c r="L10">
+        <v>90</v>
+      </c>
+      <c r="M10" s="58">
+        <v>90</v>
+      </c>
+      <c r="N10">
+        <v>9</v>
+      </c>
+      <c r="O10">
+        <v>9</v>
+      </c>
+      <c r="P10">
+        <v>9</v>
+      </c>
+      <c r="Q10">
+        <v>9</v>
+      </c>
+      <c r="R10">
+        <v>9</v>
+      </c>
+      <c r="S10">
+        <v>9</v>
+      </c>
+      <c r="T10">
+        <v>9</v>
+      </c>
+      <c r="U10">
+        <v>9</v>
+      </c>
+      <c r="V10">
+        <v>9</v>
+      </c>
+      <c r="W10" t="s">
+        <v>74</v>
+      </c>
+      <c r="X10" t="s">
+        <v>74</v>
+      </c>
+      <c r="Y10" t="s">
+        <v>74</v>
+      </c>
+      <c r="Z10">
+        <v>9</v>
+      </c>
+      <c r="AA10" s="59">
+        <v>9</v>
+      </c>
+      <c r="AB10">
+        <v>10</v>
+      </c>
+      <c r="AC10" s="56">
+        <v>44144</v>
+      </c>
+    </row>
+    <row r="11" spans="1:29">
       <c r="A11" s="51">
         <v>100</v>
       </c>
@@ -1809,10 +3280,92 @@
       <c r="F11" s="51">
         <v>10</v>
       </c>
+      <c r="G11" s="55">
+        <v>10</v>
+      </c>
+      <c r="H11">
+        <v>10</v>
+      </c>
+      <c r="I11">
+        <v>10</v>
+      </c>
+      <c r="J11">
+        <v>100</v>
+      </c>
+      <c r="K11">
+        <v>100</v>
+      </c>
+      <c r="L11">
+        <v>100</v>
+      </c>
+      <c r="M11" s="58">
+        <v>100</v>
+      </c>
+      <c r="N11">
+        <v>10</v>
+      </c>
+      <c r="O11">
+        <v>10</v>
+      </c>
+      <c r="P11">
+        <v>10</v>
+      </c>
+      <c r="Q11">
+        <v>10</v>
+      </c>
+      <c r="R11">
+        <v>10</v>
+      </c>
+      <c r="S11">
+        <v>10</v>
+      </c>
+      <c r="T11">
+        <v>10</v>
+      </c>
+      <c r="U11">
+        <v>10</v>
+      </c>
+      <c r="V11">
+        <v>10</v>
+      </c>
+      <c r="W11" t="s">
+        <v>75</v>
+      </c>
+      <c r="X11" t="s">
+        <v>75</v>
+      </c>
+      <c r="Y11" t="s">
+        <v>75</v>
+      </c>
+      <c r="Z11">
+        <v>10</v>
+      </c>
+      <c r="AA11" s="59">
+        <v>10</v>
+      </c>
+      <c r="AB11">
+        <v>10</v>
+      </c>
+      <c r="AC11" s="56">
+        <v>44145</v>
+      </c>
+    </row>
+    <row r="21" spans="19:19">
+      <c r="S21" t="s">
+        <v>83</v>
+      </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:A11">
-    <cfRule type="colorScale" priority="7">
+    <cfRule type="colorScale" priority="28">
+      <colorScale>
+        <cfvo type="num" val="1"/>
+        <cfvo type="num" val="100"/>
+        <color rgb="FFFF7128"/>
+        <color rgb="FFFFEF9C"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="30">
       <colorScale>
         <cfvo type="min" val="0"/>
         <cfvo type="percentile" val="50"/>
@@ -1822,17 +3375,9 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="colorScale" priority="5">
-      <colorScale>
-        <cfvo type="num" val="1"/>
-        <cfvo type="num" val="100"/>
-        <color rgb="FFFF7128"/>
-        <color rgb="FFFFEF9C"/>
-      </colorScale>
-    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:B11">
-    <cfRule type="colorScale" priority="6">
+    <cfRule type="colorScale" priority="29">
       <colorScale>
         <cfvo type="percentile" val="10"/>
         <cfvo type="percentile" val="50"/>
@@ -1844,7 +3389,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2:C11">
-    <cfRule type="colorScale" priority="4">
+    <cfRule type="colorScale" priority="27">
       <colorScale>
         <cfvo type="percent" val="0"/>
         <cfvo type="percent" val="50"/>
@@ -1856,7 +3401,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2:D11">
-    <cfRule type="colorScale" priority="3">
+    <cfRule type="colorScale" priority="26">
       <colorScale>
         <cfvo type="min" val="0"/>
         <cfvo type="percent" val="50"/>
@@ -1868,7 +3413,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:E11">
-    <cfRule type="colorScale" priority="2">
+    <cfRule type="colorScale" priority="25">
       <colorScale>
         <cfvo type="formula" val="$B$2"/>
         <cfvo type="formula" val="$B$6"/>
@@ -1880,7 +3425,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2:F11">
-    <cfRule type="colorScale" priority="1">
+    <cfRule type="colorScale" priority="24">
       <colorScale>
         <cfvo type="formula" val="$B$2"/>
         <cfvo type="formula" val="$B$6*4"/>
@@ -1889,6 +3434,130 @@
         <color rgb="FFFFEB84"/>
         <color rgb="FF5A8AC6"/>
       </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G2:G11">
+    <cfRule type="dataBar" priority="23">
+      <dataBar>
+        <cfvo type="min" val="0"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FF638EC6"/>
+      </dataBar>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H2:H11">
+    <cfRule type="dataBar" priority="22">
+      <dataBar showValue="0">
+        <cfvo type="min" val="0"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FF638EC6"/>
+      </dataBar>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I2:I11">
+    <cfRule type="top10" dxfId="35" priority="21" percent="1" rank="20"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J2:J11">
+    <cfRule type="top10" dxfId="34" priority="20" rank="5"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K2:K11">
+    <cfRule type="top10" dxfId="33" priority="19" bottom="1" rank="5"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L2:L11">
+    <cfRule type="aboveAverage" dxfId="32" priority="18"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M2:M11">
+    <cfRule type="aboveAverage" dxfId="31" priority="17" aboveAverage="0"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N2:N11">
+    <cfRule type="iconSet" priority="16">
+      <iconSet iconSet="3Flags" reverse="1">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="num" val="4" gte="0"/>
+        <cfvo type="num" val="8"/>
+      </iconSet>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O2:O11">
+    <cfRule type="iconSet" priority="15">
+      <iconSet iconSet="5ArrowsGray">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="percent" val="20"/>
+        <cfvo type="percent" val="40"/>
+        <cfvo type="percent" val="60"/>
+        <cfvo type="percent" val="80"/>
+      </iconSet>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P2:P11">
+    <cfRule type="iconSet" priority="14">
+      <iconSet iconSet="3Symbols2" showValue="0" reverse="1">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="percent" val="33"/>
+        <cfvo type="percent" val="67"/>
+      </iconSet>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Q2:Q11">
+    <cfRule type="cellIs" dxfId="30" priority="13" operator="greaterThan">
+      <formula>5.5</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S2:S11">
+    <cfRule type="cellIs" dxfId="29" priority="12" stopIfTrue="1" operator="equal">
+      <formula>2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="R2:R11">
+    <cfRule type="cellIs" dxfId="28" priority="11" operator="lessThan">
+      <formula>5.5</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="T2:T11">
+    <cfRule type="cellIs" dxfId="27" priority="10" operator="notEqual">
+      <formula>5</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="U2:U11">
+    <cfRule type="cellIs" dxfId="26" priority="9" operator="greaterThanOrEqual">
+      <formula>4</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="V2:V11">
+    <cfRule type="cellIs" dxfId="25" priority="8" operator="between">
+      <formula>3</formula>
+      <formula>8</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="W2:W11">
+    <cfRule type="containsText" dxfId="24" priority="7" operator="containsText" text="land">
+      <formula>NOT(ISERROR(SEARCH("land",W2)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Y2:Y11">
+    <cfRule type="beginsWith" dxfId="23" priority="6" operator="beginsWith" text="S">
+      <formula>LEFT(Y2,1)="S"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="X2:X11">
+    <cfRule type="endsWith" dxfId="22" priority="5" operator="endsWith" text="ia">
+      <formula>RIGHT(X2,2)="ia"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Z2:Z11">
+    <cfRule type="duplicateValues" dxfId="21" priority="4"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AA2:AA11">
+    <cfRule type="cellIs" dxfId="18" priority="3" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AB2:AB11">
+    <cfRule type="uniqueValues" dxfId="20" priority="2"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AC2:AC11">
+    <cfRule type="timePeriod" dxfId="19" priority="1" timePeriod="lastWeek">
+      <formula>AND(TODAY()-ROUNDDOWN(AC2,0)&gt;=(WEEKDAY(TODAY())),TODAY()-ROUNDDOWN(AC2,0)&lt;(WEEKDAY(TODAY())+7))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added test cases for data bar, icon set, and others (issue #5). Cleaned up style setting code. Patched bugs in ExcelJS.
</commit_message>
<xml_diff>
--- a/backend/test/assets/sample.xlsx
+++ b/backend/test/assets/sample.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4507"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Text (with styles)" sheetId="2" r:id="rId1"/>
@@ -293,9 +293,6 @@
     <t>Data bar 2</t>
   </si>
   <si>
-    <t>Top 10%</t>
-  </si>
-  <si>
     <t>Top 5</t>
   </si>
   <si>
@@ -305,9 +302,6 @@
     <t>Above avg</t>
   </si>
   <si>
-    <t>Below Avg</t>
-  </si>
-  <si>
     <t>Icon set 1</t>
   </si>
   <si>
@@ -387,6 +381,12 @@
   </si>
   <si>
     <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Top 20%</t>
+  </si>
+  <si>
+    <t>Below avg</t>
   </si>
 </sst>
 </file>
@@ -857,21 +857,29 @@
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="20" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="54">
+  <dxfs count="72">
     <dxf>
       <font>
         <condense val="0"/>
@@ -900,7 +908,7 @@
       <font>
         <color rgb="FFFFFF00"/>
       </font>
-      <numFmt numFmtId="14" formatCode="0.00%"/>
+      <numFmt numFmtId="168" formatCode="0.00_);[Red]\(0.00\)"/>
       <fill>
         <patternFill>
           <bgColor rgb="FF00B050"/>
@@ -1094,6 +1102,30 @@
     </dxf>
     <dxf>
       <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FFFFFF00"/>
       </font>
       <numFmt numFmtId="168" formatCode="0.00_);[Red]\(0.00\)"/>
@@ -1116,14 +1148,210 @@
       </fill>
     </dxf>
     <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFFFF00"/>
+      </font>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1917,9 +2145,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C33"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -2192,10 +2418,10 @@
       </c>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3" s="57" t="s">
+      <c r="A3" s="54" t="s">
         <v>30</v>
       </c>
-      <c r="B3" s="57"/>
+      <c r="B3" s="54"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2350,8 +2576,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AC21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="R1" workbookViewId="0">
-      <selection activeCell="AA2" sqref="AA2:AA11"/>
+    <sheetView topLeftCell="P1" workbookViewId="0">
+      <selection activeCell="P2" sqref="P2:P11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2397,67 +2623,67 @@
         <v>51</v>
       </c>
       <c r="I1" s="26" t="s">
+        <v>82</v>
+      </c>
+      <c r="J1" s="26" t="s">
         <v>52</v>
       </c>
-      <c r="J1" s="26" t="s">
+      <c r="K1" s="26" t="s">
         <v>53</v>
       </c>
-      <c r="K1" s="26" t="s">
+      <c r="L1" s="26" t="s">
         <v>54</v>
       </c>
-      <c r="L1" s="26" t="s">
+      <c r="M1" s="26" t="s">
+        <v>83</v>
+      </c>
+      <c r="N1" s="26" t="s">
         <v>55</v>
       </c>
-      <c r="M1" s="26" t="s">
+      <c r="O1" s="26" t="s">
         <v>56</v>
       </c>
-      <c r="N1" s="26" t="s">
+      <c r="P1" s="26" t="s">
         <v>57</v>
       </c>
-      <c r="O1" s="26" t="s">
+      <c r="Q1" s="26" t="s">
         <v>58</v>
       </c>
-      <c r="P1" s="26" t="s">
+      <c r="R1" s="26" t="s">
         <v>59</v>
       </c>
-      <c r="Q1" s="26" t="s">
+      <c r="S1" s="26" t="s">
         <v>60</v>
       </c>
-      <c r="R1" s="26" t="s">
+      <c r="T1" s="26" t="s">
         <v>61</v>
       </c>
-      <c r="S1" s="26" t="s">
+      <c r="U1" s="26" t="s">
         <v>62</v>
       </c>
-      <c r="T1" s="26" t="s">
+      <c r="V1" s="26" t="s">
         <v>63</v>
       </c>
-      <c r="U1" s="26" t="s">
-        <v>64</v>
-      </c>
-      <c r="V1" s="26" t="s">
-        <v>65</v>
-      </c>
       <c r="W1" s="26" t="s">
+        <v>74</v>
+      </c>
+      <c r="X1" s="26" t="s">
+        <v>75</v>
+      </c>
+      <c r="Y1" s="26" t="s">
         <v>76</v>
       </c>
-      <c r="X1" s="26" t="s">
+      <c r="Z1" s="26" t="s">
         <v>77</v>
       </c>
-      <c r="Y1" s="26" t="s">
+      <c r="AA1" s="26" t="s">
         <v>78</v>
       </c>
-      <c r="Z1" s="26" t="s">
+      <c r="AB1" s="26" t="s">
         <v>79</v>
       </c>
-      <c r="AA1" s="26" t="s">
+      <c r="AC1" s="26" t="s">
         <v>80</v>
-      </c>
-      <c r="AB1" s="26" t="s">
-        <v>81</v>
-      </c>
-      <c r="AC1" s="26" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="2" spans="1:29">
@@ -2479,73 +2705,73 @@
       <c r="F2" s="51">
         <v>1</v>
       </c>
-      <c r="G2">
+      <c r="G2" s="46">
         <v>1</v>
       </c>
-      <c r="H2">
+      <c r="H2" s="46">
+        <v>5</v>
+      </c>
+      <c r="I2" s="46">
         <v>1</v>
       </c>
-      <c r="I2">
+      <c r="J2" s="46">
+        <v>10</v>
+      </c>
+      <c r="K2" s="46">
+        <v>10</v>
+      </c>
+      <c r="L2" s="46">
+        <v>10</v>
+      </c>
+      <c r="M2" s="55">
+        <v>-10</v>
+      </c>
+      <c r="N2" s="46">
         <v>1</v>
       </c>
-      <c r="J2">
+      <c r="O2" s="46">
+        <v>1</v>
+      </c>
+      <c r="P2" s="46">
+        <v>1</v>
+      </c>
+      <c r="Q2" s="46">
+        <v>1</v>
+      </c>
+      <c r="R2" s="46">
+        <v>1</v>
+      </c>
+      <c r="S2" s="46">
+        <v>1</v>
+      </c>
+      <c r="T2" s="46">
+        <v>1</v>
+      </c>
+      <c r="U2" s="46">
+        <v>1</v>
+      </c>
+      <c r="V2" s="46">
+        <v>1</v>
+      </c>
+      <c r="W2" s="46" t="s">
+        <v>64</v>
+      </c>
+      <c r="X2" s="46" t="s">
+        <v>64</v>
+      </c>
+      <c r="Y2" s="46" t="s">
+        <v>64</v>
+      </c>
+      <c r="Z2" s="46">
+        <v>1</v>
+      </c>
+      <c r="AA2" s="56">
+        <v>1</v>
+      </c>
+      <c r="AB2" s="46">
         <v>10</v>
       </c>
-      <c r="K2">
-        <v>10</v>
-      </c>
-      <c r="L2">
-        <v>10</v>
-      </c>
-      <c r="M2" s="58">
-        <v>-10</v>
-      </c>
-      <c r="N2">
-        <v>1</v>
-      </c>
-      <c r="O2">
-        <v>1</v>
-      </c>
-      <c r="P2">
-        <v>1</v>
-      </c>
-      <c r="Q2">
-        <v>1</v>
-      </c>
-      <c r="R2">
-        <v>1</v>
-      </c>
-      <c r="S2">
-        <v>1</v>
-      </c>
-      <c r="T2">
-        <v>1</v>
-      </c>
-      <c r="U2">
-        <v>1</v>
-      </c>
-      <c r="V2">
-        <v>1</v>
-      </c>
-      <c r="W2" t="s">
-        <v>66</v>
-      </c>
-      <c r="X2" t="s">
-        <v>66</v>
-      </c>
-      <c r="Y2" t="s">
-        <v>66</v>
-      </c>
-      <c r="Z2">
-        <v>1</v>
-      </c>
-      <c r="AA2" s="59">
-        <v>1</v>
-      </c>
-      <c r="AB2">
-        <v>10</v>
-      </c>
-      <c r="AC2" s="56">
+      <c r="AC2" s="57">
         <v>44136</v>
       </c>
     </row>
@@ -2568,73 +2794,73 @@
       <c r="F3" s="51">
         <v>2</v>
       </c>
-      <c r="G3">
+      <c r="G3" s="46">
         <v>2</v>
       </c>
-      <c r="H3">
+      <c r="H3" s="46">
+        <v>6</v>
+      </c>
+      <c r="I3" s="46">
         <v>2</v>
       </c>
-      <c r="I3">
+      <c r="J3" s="46">
+        <v>20</v>
+      </c>
+      <c r="K3" s="46">
+        <v>20</v>
+      </c>
+      <c r="L3" s="46">
+        <v>20</v>
+      </c>
+      <c r="M3" s="55">
+        <v>20</v>
+      </c>
+      <c r="N3" s="46">
         <v>2</v>
       </c>
-      <c r="J3">
-        <v>20</v>
-      </c>
-      <c r="K3">
-        <v>20</v>
-      </c>
-      <c r="L3">
-        <v>20</v>
-      </c>
-      <c r="M3" s="58">
-        <v>20</v>
-      </c>
-      <c r="N3">
+      <c r="O3" s="46">
         <v>2</v>
       </c>
-      <c r="O3">
+      <c r="P3" s="46">
         <v>2</v>
       </c>
-      <c r="P3">
+      <c r="Q3" s="46">
         <v>2</v>
       </c>
-      <c r="Q3">
+      <c r="R3" s="46">
         <v>2</v>
       </c>
-      <c r="R3">
+      <c r="S3" s="46">
         <v>2</v>
       </c>
-      <c r="S3">
+      <c r="T3" s="46">
         <v>2</v>
       </c>
-      <c r="T3">
+      <c r="U3" s="46">
         <v>2</v>
       </c>
-      <c r="U3">
+      <c r="V3" s="46">
         <v>2</v>
       </c>
-      <c r="V3">
+      <c r="W3" s="46" t="s">
+        <v>65</v>
+      </c>
+      <c r="X3" s="46" t="s">
+        <v>65</v>
+      </c>
+      <c r="Y3" s="46" t="s">
+        <v>65</v>
+      </c>
+      <c r="Z3" s="46">
         <v>2</v>
       </c>
-      <c r="W3" t="s">
-        <v>67</v>
-      </c>
-      <c r="X3" t="s">
-        <v>67</v>
-      </c>
-      <c r="Y3" t="s">
-        <v>67</v>
-      </c>
-      <c r="Z3">
+      <c r="AA3" s="56">
         <v>2</v>
       </c>
-      <c r="AA3" s="59">
-        <v>2</v>
-      </c>
-      <c r="AB3">
+      <c r="AB3" s="46">
         <v>10</v>
       </c>
-      <c r="AC3" s="56">
+      <c r="AC3" s="57">
         <v>44137</v>
       </c>
     </row>
@@ -2657,73 +2883,73 @@
       <c r="F4" s="51">
         <v>3</v>
       </c>
-      <c r="G4">
+      <c r="G4" s="46">
         <v>3</v>
       </c>
-      <c r="H4">
+      <c r="H4" s="46">
+        <v>7</v>
+      </c>
+      <c r="I4" s="46">
         <v>3</v>
       </c>
-      <c r="I4">
+      <c r="J4" s="46">
+        <v>30</v>
+      </c>
+      <c r="K4" s="46">
+        <v>30</v>
+      </c>
+      <c r="L4" s="46">
+        <v>30</v>
+      </c>
+      <c r="M4" s="55">
+        <v>30</v>
+      </c>
+      <c r="N4" s="46">
         <v>3</v>
       </c>
-      <c r="J4">
-        <v>30</v>
-      </c>
-      <c r="K4">
-        <v>30</v>
-      </c>
-      <c r="L4">
-        <v>30</v>
-      </c>
-      <c r="M4" s="58">
-        <v>30</v>
-      </c>
-      <c r="N4">
+      <c r="O4" s="46">
         <v>3</v>
       </c>
-      <c r="O4">
+      <c r="P4" s="46">
         <v>3</v>
       </c>
-      <c r="P4">
+      <c r="Q4" s="46">
         <v>3</v>
       </c>
-      <c r="Q4">
+      <c r="R4" s="46">
         <v>3</v>
       </c>
-      <c r="R4">
+      <c r="S4" s="46">
         <v>3</v>
       </c>
-      <c r="S4">
+      <c r="T4" s="46">
         <v>3</v>
       </c>
-      <c r="T4">
+      <c r="U4" s="46">
         <v>3</v>
       </c>
-      <c r="U4">
+      <c r="V4" s="46">
         <v>3</v>
       </c>
-      <c r="V4">
+      <c r="W4" s="46" t="s">
+        <v>66</v>
+      </c>
+      <c r="X4" s="46" t="s">
+        <v>66</v>
+      </c>
+      <c r="Y4" s="46" t="s">
+        <v>66</v>
+      </c>
+      <c r="Z4" s="46">
         <v>3</v>
       </c>
-      <c r="W4" t="s">
-        <v>68</v>
-      </c>
-      <c r="X4" t="s">
-        <v>68</v>
-      </c>
-      <c r="Y4" t="s">
-        <v>68</v>
-      </c>
-      <c r="Z4">
-        <v>3</v>
-      </c>
-      <c r="AA4" s="59">
+      <c r="AA4" s="56">
         <v>-3</v>
       </c>
-      <c r="AB4">
+      <c r="AB4" s="46">
         <v>11</v>
       </c>
-      <c r="AC4" s="56">
+      <c r="AC4" s="57">
         <v>44138</v>
       </c>
     </row>
@@ -2746,73 +2972,73 @@
       <c r="F5" s="51">
         <v>4</v>
       </c>
-      <c r="G5">
+      <c r="G5" s="46">
         <v>4</v>
       </c>
-      <c r="H5">
+      <c r="H5" s="46">
+        <v>8</v>
+      </c>
+      <c r="I5" s="46">
         <v>4</v>
       </c>
-      <c r="I5">
+      <c r="J5" s="46">
+        <v>40</v>
+      </c>
+      <c r="K5" s="46">
+        <v>40</v>
+      </c>
+      <c r="L5" s="46">
+        <v>40</v>
+      </c>
+      <c r="M5" s="55">
+        <v>40</v>
+      </c>
+      <c r="N5" s="46">
         <v>4</v>
       </c>
-      <c r="J5">
-        <v>40</v>
-      </c>
-      <c r="K5">
-        <v>40</v>
-      </c>
-      <c r="L5">
-        <v>40</v>
-      </c>
-      <c r="M5" s="58">
-        <v>40</v>
-      </c>
-      <c r="N5">
+      <c r="O5" s="46">
         <v>4</v>
       </c>
-      <c r="O5">
+      <c r="P5" s="46">
         <v>4</v>
       </c>
-      <c r="P5">
+      <c r="Q5" s="46">
         <v>4</v>
       </c>
-      <c r="Q5">
+      <c r="R5" s="46">
         <v>4</v>
       </c>
-      <c r="R5">
+      <c r="S5" s="46">
         <v>4</v>
       </c>
-      <c r="S5">
+      <c r="T5" s="46">
         <v>4</v>
       </c>
-      <c r="T5">
+      <c r="U5" s="46">
         <v>4</v>
       </c>
-      <c r="U5">
+      <c r="V5" s="46">
         <v>4</v>
       </c>
-      <c r="V5">
+      <c r="W5" s="46" t="s">
+        <v>67</v>
+      </c>
+      <c r="X5" s="46" t="s">
+        <v>67</v>
+      </c>
+      <c r="Y5" s="46" t="s">
+        <v>67</v>
+      </c>
+      <c r="Z5" s="46">
         <v>4</v>
       </c>
-      <c r="W5" t="s">
-        <v>69</v>
-      </c>
-      <c r="X5" t="s">
-        <v>69</v>
-      </c>
-      <c r="Y5" t="s">
-        <v>69</v>
-      </c>
-      <c r="Z5">
-        <v>4</v>
-      </c>
-      <c r="AA5" s="59">
+      <c r="AA5" s="56">
         <v>-4</v>
       </c>
-      <c r="AB5">
+      <c r="AB5" s="46">
         <v>10</v>
       </c>
-      <c r="AC5" s="56">
+      <c r="AC5" s="57">
         <v>44139</v>
       </c>
     </row>
@@ -2835,73 +3061,73 @@
       <c r="F6" s="51">
         <v>5</v>
       </c>
-      <c r="G6">
+      <c r="G6" s="46">
         <v>5</v>
       </c>
-      <c r="H6">
+      <c r="H6" s="46">
+        <v>9</v>
+      </c>
+      <c r="I6" s="46">
         <v>5</v>
       </c>
-      <c r="I6">
+      <c r="J6" s="46">
+        <v>50</v>
+      </c>
+      <c r="K6" s="46">
+        <v>50</v>
+      </c>
+      <c r="L6" s="46">
+        <v>50</v>
+      </c>
+      <c r="M6" s="55">
+        <v>50</v>
+      </c>
+      <c r="N6" s="46">
         <v>5</v>
       </c>
-      <c r="J6">
-        <v>50</v>
-      </c>
-      <c r="K6">
-        <v>50</v>
-      </c>
-      <c r="L6">
-        <v>50</v>
-      </c>
-      <c r="M6" s="58">
-        <v>50</v>
-      </c>
-      <c r="N6">
+      <c r="O6" s="46">
         <v>5</v>
       </c>
-      <c r="O6">
+      <c r="P6" s="46">
         <v>5</v>
       </c>
-      <c r="P6">
+      <c r="Q6" s="46">
         <v>5</v>
       </c>
-      <c r="Q6">
+      <c r="R6" s="46">
         <v>5</v>
       </c>
-      <c r="R6">
+      <c r="S6" s="46">
         <v>5</v>
       </c>
-      <c r="S6">
+      <c r="T6" s="46">
         <v>5</v>
       </c>
-      <c r="T6">
+      <c r="U6" s="46">
         <v>5</v>
       </c>
-      <c r="U6">
+      <c r="V6" s="46">
         <v>5</v>
       </c>
-      <c r="V6">
-        <v>5</v>
-      </c>
-      <c r="W6" t="s">
-        <v>70</v>
-      </c>
-      <c r="X6" t="s">
-        <v>70</v>
-      </c>
-      <c r="Y6" t="s">
-        <v>70</v>
-      </c>
-      <c r="Z6">
+      <c r="W6" s="46" t="s">
+        <v>68</v>
+      </c>
+      <c r="X6" s="46" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y6" s="46" t="s">
+        <v>68</v>
+      </c>
+      <c r="Z6" s="46">
         <v>10</v>
       </c>
-      <c r="AA6" s="59">
+      <c r="AA6" s="56">
         <v>-5</v>
       </c>
-      <c r="AB6">
+      <c r="AB6" s="46">
         <v>10</v>
       </c>
-      <c r="AC6" s="56">
+      <c r="AC6" s="57">
         <v>44140</v>
       </c>
     </row>
@@ -2924,73 +3150,73 @@
       <c r="F7" s="51">
         <v>6</v>
       </c>
-      <c r="G7">
+      <c r="G7" s="46">
         <v>6</v>
       </c>
-      <c r="H7" s="54">
+      <c r="H7" s="58">
+        <v>10</v>
+      </c>
+      <c r="I7" s="46">
         <v>6</v>
       </c>
-      <c r="I7">
+      <c r="J7" s="46">
+        <v>60</v>
+      </c>
+      <c r="K7" s="46">
+        <v>60</v>
+      </c>
+      <c r="L7" s="46">
+        <v>60</v>
+      </c>
+      <c r="M7" s="55">
+        <v>60</v>
+      </c>
+      <c r="N7" s="46">
         <v>6</v>
       </c>
-      <c r="J7">
-        <v>60</v>
-      </c>
-      <c r="K7">
-        <v>60</v>
-      </c>
-      <c r="L7">
-        <v>60</v>
-      </c>
-      <c r="M7" s="58">
-        <v>60</v>
-      </c>
-      <c r="N7">
+      <c r="O7" s="46">
         <v>6</v>
       </c>
-      <c r="O7">
+      <c r="P7" s="46">
         <v>6</v>
       </c>
-      <c r="P7">
+      <c r="Q7" s="46">
         <v>6</v>
       </c>
-      <c r="Q7">
+      <c r="R7" s="46">
         <v>6</v>
       </c>
-      <c r="R7">
+      <c r="S7" s="46">
         <v>6</v>
       </c>
-      <c r="S7">
+      <c r="T7" s="46">
         <v>6</v>
       </c>
-      <c r="T7">
+      <c r="U7" s="46">
         <v>6</v>
       </c>
-      <c r="U7">
+      <c r="V7" s="46">
         <v>6</v>
       </c>
-      <c r="V7">
+      <c r="W7" s="46" t="s">
+        <v>69</v>
+      </c>
+      <c r="X7" s="46" t="s">
+        <v>69</v>
+      </c>
+      <c r="Y7" s="46" t="s">
+        <v>69</v>
+      </c>
+      <c r="Z7" s="46">
         <v>6</v>
       </c>
-      <c r="W7" t="s">
-        <v>71</v>
-      </c>
-      <c r="X7" t="s">
-        <v>71</v>
-      </c>
-      <c r="Y7" t="s">
-        <v>71</v>
-      </c>
-      <c r="Z7">
+      <c r="AA7" s="56">
         <v>6</v>
       </c>
-      <c r="AA7" s="59">
-        <v>6</v>
-      </c>
-      <c r="AB7">
+      <c r="AB7" s="46">
         <v>20</v>
       </c>
-      <c r="AC7" s="56">
+      <c r="AC7" s="57">
         <v>44141</v>
       </c>
     </row>
@@ -3013,73 +3239,73 @@
       <c r="F8" s="51">
         <v>7</v>
       </c>
-      <c r="G8">
+      <c r="G8" s="46">
         <v>7</v>
       </c>
-      <c r="H8">
+      <c r="H8" s="46">
+        <v>11</v>
+      </c>
+      <c r="I8" s="46">
         <v>7</v>
       </c>
-      <c r="I8">
+      <c r="J8" s="46">
+        <v>70</v>
+      </c>
+      <c r="K8" s="46">
+        <v>70</v>
+      </c>
+      <c r="L8" s="46">
+        <v>70</v>
+      </c>
+      <c r="M8" s="55">
+        <v>70</v>
+      </c>
+      <c r="N8" s="46">
         <v>7</v>
       </c>
-      <c r="J8">
+      <c r="O8" s="46">
+        <v>7</v>
+      </c>
+      <c r="P8" s="46">
+        <v>7</v>
+      </c>
+      <c r="Q8" s="46">
+        <v>7</v>
+      </c>
+      <c r="R8" s="46">
+        <v>7</v>
+      </c>
+      <c r="S8" s="46">
+        <v>7</v>
+      </c>
+      <c r="T8" s="46">
+        <v>7</v>
+      </c>
+      <c r="U8" s="46">
+        <v>7</v>
+      </c>
+      <c r="V8" s="46">
+        <v>7</v>
+      </c>
+      <c r="W8" s="46" t="s">
         <v>70</v>
       </c>
-      <c r="K8">
+      <c r="X8" s="46" t="s">
         <v>70</v>
       </c>
-      <c r="L8">
+      <c r="Y8" s="46" t="s">
         <v>70</v>
       </c>
-      <c r="M8" s="58">
-        <v>70</v>
-      </c>
-      <c r="N8">
+      <c r="Z8" s="46">
         <v>7</v>
       </c>
-      <c r="O8">
+      <c r="AA8" s="56">
         <v>7</v>
       </c>
-      <c r="P8">
-        <v>7</v>
-      </c>
-      <c r="Q8">
-        <v>7</v>
-      </c>
-      <c r="R8">
-        <v>7</v>
-      </c>
-      <c r="S8">
-        <v>7</v>
-      </c>
-      <c r="T8">
-        <v>7</v>
-      </c>
-      <c r="U8">
-        <v>7</v>
-      </c>
-      <c r="V8">
-        <v>7</v>
-      </c>
-      <c r="W8" t="s">
-        <v>72</v>
-      </c>
-      <c r="X8" t="s">
-        <v>72</v>
-      </c>
-      <c r="Y8" t="s">
-        <v>72</v>
-      </c>
-      <c r="Z8">
-        <v>7</v>
-      </c>
-      <c r="AA8" s="59">
-        <v>7</v>
-      </c>
-      <c r="AB8">
+      <c r="AB8" s="46">
         <v>20</v>
       </c>
-      <c r="AC8" s="56">
+      <c r="AC8" s="57">
         <v>44142</v>
       </c>
     </row>
@@ -3102,73 +3328,73 @@
       <c r="F9" s="51">
         <v>8</v>
       </c>
-      <c r="G9">
+      <c r="G9" s="46">
         <v>8</v>
       </c>
-      <c r="H9">
+      <c r="H9" s="46">
+        <v>12</v>
+      </c>
+      <c r="I9" s="46">
         <v>8</v>
       </c>
-      <c r="I9">
+      <c r="J9" s="46">
+        <v>80</v>
+      </c>
+      <c r="K9" s="46">
+        <v>80</v>
+      </c>
+      <c r="L9" s="46">
+        <v>80</v>
+      </c>
+      <c r="M9" s="55">
+        <v>80</v>
+      </c>
+      <c r="N9" s="46">
         <v>8</v>
       </c>
-      <c r="J9">
-        <v>80</v>
-      </c>
-      <c r="K9">
-        <v>80</v>
-      </c>
-      <c r="L9">
-        <v>80</v>
-      </c>
-      <c r="M9" s="58">
-        <v>80</v>
-      </c>
-      <c r="N9">
+      <c r="O9" s="46">
         <v>8</v>
       </c>
-      <c r="O9">
+      <c r="P9" s="46">
         <v>8</v>
       </c>
-      <c r="P9">
+      <c r="Q9" s="46">
         <v>8</v>
       </c>
-      <c r="Q9">
+      <c r="R9" s="46">
         <v>8</v>
       </c>
-      <c r="R9">
+      <c r="S9" s="46">
         <v>8</v>
       </c>
-      <c r="S9">
+      <c r="T9" s="46">
         <v>8</v>
       </c>
-      <c r="T9">
+      <c r="U9" s="46">
         <v>8</v>
       </c>
-      <c r="U9">
+      <c r="V9" s="46">
         <v>8</v>
       </c>
-      <c r="V9">
+      <c r="W9" s="46" t="s">
+        <v>71</v>
+      </c>
+      <c r="X9" s="46" t="s">
+        <v>71</v>
+      </c>
+      <c r="Y9" s="46" t="s">
+        <v>71</v>
+      </c>
+      <c r="Z9" s="46">
+        <v>10</v>
+      </c>
+      <c r="AA9" s="56">
         <v>8</v>
       </c>
-      <c r="W9" t="s">
-        <v>73</v>
-      </c>
-      <c r="X9" t="s">
-        <v>73</v>
-      </c>
-      <c r="Y9" t="s">
-        <v>73</v>
-      </c>
-      <c r="Z9">
+      <c r="AB9" s="46">
         <v>10</v>
       </c>
-      <c r="AA9" s="59">
-        <v>8</v>
-      </c>
-      <c r="AB9">
-        <v>10</v>
-      </c>
-      <c r="AC9" s="56">
+      <c r="AC9" s="57">
         <v>44143</v>
       </c>
     </row>
@@ -3191,73 +3417,73 @@
       <c r="F10" s="51">
         <v>9</v>
       </c>
-      <c r="G10">
+      <c r="G10" s="46">
         <v>9</v>
       </c>
-      <c r="H10">
+      <c r="H10" s="46">
+        <v>13</v>
+      </c>
+      <c r="I10" s="46">
         <v>9</v>
       </c>
-      <c r="I10">
+      <c r="J10" s="46">
+        <v>90</v>
+      </c>
+      <c r="K10" s="46">
+        <v>90</v>
+      </c>
+      <c r="L10" s="46">
+        <v>90</v>
+      </c>
+      <c r="M10" s="55">
+        <v>90</v>
+      </c>
+      <c r="N10" s="46">
         <v>9</v>
       </c>
-      <c r="J10">
-        <v>90</v>
-      </c>
-      <c r="K10">
-        <v>90</v>
-      </c>
-      <c r="L10">
-        <v>90</v>
-      </c>
-      <c r="M10" s="58">
-        <v>90</v>
-      </c>
-      <c r="N10">
+      <c r="O10" s="46">
         <v>9</v>
       </c>
-      <c r="O10">
+      <c r="P10" s="46">
         <v>9</v>
       </c>
-      <c r="P10">
+      <c r="Q10" s="46">
         <v>9</v>
       </c>
-      <c r="Q10">
+      <c r="R10" s="46">
         <v>9</v>
       </c>
-      <c r="R10">
+      <c r="S10" s="46">
         <v>9</v>
       </c>
-      <c r="S10">
+      <c r="T10" s="46">
         <v>9</v>
       </c>
-      <c r="T10">
+      <c r="U10" s="46">
         <v>9</v>
       </c>
-      <c r="U10">
+      <c r="V10" s="46">
         <v>9</v>
       </c>
-      <c r="V10">
+      <c r="W10" s="46" t="s">
+        <v>72</v>
+      </c>
+      <c r="X10" s="46" t="s">
+        <v>72</v>
+      </c>
+      <c r="Y10" s="46" t="s">
+        <v>72</v>
+      </c>
+      <c r="Z10" s="46">
         <v>9</v>
       </c>
-      <c r="W10" t="s">
-        <v>74</v>
-      </c>
-      <c r="X10" t="s">
-        <v>74</v>
-      </c>
-      <c r="Y10" t="s">
-        <v>74</v>
-      </c>
-      <c r="Z10">
+      <c r="AA10" s="56">
         <v>9</v>
       </c>
-      <c r="AA10" s="59">
-        <v>9</v>
-      </c>
-      <c r="AB10">
+      <c r="AB10" s="46">
         <v>10</v>
       </c>
-      <c r="AC10" s="56">
+      <c r="AC10" s="57">
         <v>44144</v>
       </c>
     </row>
@@ -3280,79 +3506,79 @@
       <c r="F11" s="51">
         <v>10</v>
       </c>
-      <c r="G11" s="55">
+      <c r="G11" s="59">
         <v>10</v>
       </c>
-      <c r="H11">
+      <c r="H11" s="46">
+        <v>14</v>
+      </c>
+      <c r="I11" s="46">
         <v>10</v>
       </c>
-      <c r="I11">
+      <c r="J11" s="46">
+        <v>100</v>
+      </c>
+      <c r="K11" s="46">
+        <v>100</v>
+      </c>
+      <c r="L11" s="46">
+        <v>100</v>
+      </c>
+      <c r="M11" s="55">
+        <v>100</v>
+      </c>
+      <c r="N11" s="46">
         <v>10</v>
       </c>
-      <c r="J11">
-        <v>100</v>
-      </c>
-      <c r="K11">
-        <v>100</v>
-      </c>
-      <c r="L11">
-        <v>100</v>
-      </c>
-      <c r="M11" s="58">
-        <v>100</v>
-      </c>
-      <c r="N11">
+      <c r="O11" s="46">
         <v>10</v>
       </c>
-      <c r="O11">
+      <c r="P11" s="46">
         <v>10</v>
       </c>
-      <c r="P11">
+      <c r="Q11" s="46">
         <v>10</v>
       </c>
-      <c r="Q11">
+      <c r="R11" s="46">
         <v>10</v>
       </c>
-      <c r="R11">
+      <c r="S11" s="46">
         <v>10</v>
       </c>
-      <c r="S11">
+      <c r="T11" s="46">
         <v>10</v>
       </c>
-      <c r="T11">
+      <c r="U11" s="46">
         <v>10</v>
       </c>
-      <c r="U11">
+      <c r="V11" s="46">
         <v>10</v>
       </c>
-      <c r="V11">
+      <c r="W11" s="46" t="s">
+        <v>73</v>
+      </c>
+      <c r="X11" s="46" t="s">
+        <v>73</v>
+      </c>
+      <c r="Y11" s="46" t="s">
+        <v>73</v>
+      </c>
+      <c r="Z11" s="46">
         <v>10</v>
       </c>
-      <c r="W11" t="s">
-        <v>75</v>
-      </c>
-      <c r="X11" t="s">
-        <v>75</v>
-      </c>
-      <c r="Y11" t="s">
-        <v>75</v>
-      </c>
-      <c r="Z11">
+      <c r="AA11" s="56">
         <v>10</v>
       </c>
-      <c r="AA11" s="59">
+      <c r="AB11" s="46">
         <v>10</v>
       </c>
-      <c r="AB11">
-        <v>10</v>
-      </c>
-      <c r="AC11" s="56">
+      <c r="AC11" s="57">
         <v>44145</v>
       </c>
     </row>
     <row r="21" spans="19:19">
       <c r="S21" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
   </sheetData>
@@ -3491,7 +3717,7 @@
   </conditionalFormatting>
   <conditionalFormatting sqref="P2:P11">
     <cfRule type="iconSet" priority="14">
-      <iconSet iconSet="3Symbols2" showValue="0" reverse="1">
+      <iconSet iconSet="3Symbols2" showValue="0">
         <cfvo type="percent" val="0"/>
         <cfvo type="percent" val="33"/>
         <cfvo type="percent" val="67"/>
@@ -3548,15 +3774,15 @@
     <cfRule type="duplicateValues" dxfId="21" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA2:AA11">
-    <cfRule type="cellIs" dxfId="18" priority="3" operator="lessThan">
+    <cfRule type="cellIs" dxfId="20" priority="3" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB2:AB11">
-    <cfRule type="uniqueValues" dxfId="20" priority="2"/>
+    <cfRule type="uniqueValues" dxfId="19" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="AC2:AC11">
-    <cfRule type="timePeriod" dxfId="19" priority="1" timePeriod="lastWeek">
+    <cfRule type="timePeriod" dxfId="18" priority="1" timePeriod="lastWeek">
       <formula>AND(TODAY()-ROUNDDOWN(AC2,0)&gt;=(WEEKDAY(TODAY())),TODAY()-ROUNDDOWN(AC2,0)&lt;(WEEKDAY(TODAY())+7))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Implemented conditional styling by uniqueness (issue #5).
</commit_message>
<xml_diff>
--- a/backend/test/assets/sample.xlsx
+++ b/backend/test/assets/sample.xlsx
@@ -393,12 +393,13 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="5">
+  <numFmts count="6">
     <numFmt numFmtId="164" formatCode="[$$-409]#,##0.0;[Red]\-[$$-409]#,##0.0"/>
     <numFmt numFmtId="165" formatCode="#,##0.00\ [$PLN];[Red]\-#,##0.00\ [$PLN]"/>
     <numFmt numFmtId="166" formatCode="mm/dd/yy;@"/>
     <numFmt numFmtId="168" formatCode="0.00_);[Red]\(0.00\)"/>
     <numFmt numFmtId="169" formatCode="&quot;$&quot;#,##0.00"/>
+    <numFmt numFmtId="171" formatCode="\T\o\p\ @"/>
   </numFmts>
   <fonts count="9">
     <font>
@@ -770,7 +771,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -874,6 +875,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2576,8 +2580,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AC21"/>
   <sheetViews>
-    <sheetView topLeftCell="P1" workbookViewId="0">
-      <selection activeCell="P2" sqref="P2:P11"/>
+    <sheetView topLeftCell="O1" workbookViewId="0">
+      <selection activeCell="Q13" sqref="Q13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2591,9 +2595,10 @@
     <col min="7" max="7" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="23" max="25" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="25" max="27" width="14.42578125" bestFit="1" customWidth="1"/>
     <col min="29" max="29" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2647,40 +2652,40 @@
         <v>57</v>
       </c>
       <c r="Q1" s="26" t="s">
+        <v>77</v>
+      </c>
+      <c r="R1" s="26" t="s">
+        <v>79</v>
+      </c>
+      <c r="S1" s="26" t="s">
         <v>58</v>
       </c>
-      <c r="R1" s="26" t="s">
+      <c r="T1" s="26" t="s">
         <v>59</v>
       </c>
-      <c r="S1" s="26" t="s">
+      <c r="U1" s="26" t="s">
         <v>60</v>
       </c>
-      <c r="T1" s="26" t="s">
+      <c r="V1" s="26" t="s">
         <v>61</v>
       </c>
-      <c r="U1" s="26" t="s">
+      <c r="W1" s="26" t="s">
         <v>62</v>
       </c>
-      <c r="V1" s="26" t="s">
+      <c r="X1" s="26" t="s">
         <v>63</v>
       </c>
-      <c r="W1" s="26" t="s">
+      <c r="Y1" s="26" t="s">
         <v>74</v>
       </c>
-      <c r="X1" s="26" t="s">
+      <c r="Z1" s="26" t="s">
         <v>75</v>
       </c>
-      <c r="Y1" s="26" t="s">
+      <c r="AA1" s="26" t="s">
         <v>76</v>
       </c>
-      <c r="Z1" s="26" t="s">
-        <v>77</v>
-      </c>
-      <c r="AA1" s="26" t="s">
+      <c r="AB1" s="26" t="s">
         <v>78</v>
-      </c>
-      <c r="AB1" s="26" t="s">
-        <v>79</v>
       </c>
       <c r="AC1" s="26" t="s">
         <v>80</v>
@@ -2739,7 +2744,7 @@
         <v>1</v>
       </c>
       <c r="R2" s="46">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S2" s="46">
         <v>1</v>
@@ -2753,23 +2758,23 @@
       <c r="V2" s="46">
         <v>1</v>
       </c>
-      <c r="W2" s="46" t="s">
-        <v>64</v>
-      </c>
-      <c r="X2" s="46" t="s">
-        <v>64</v>
+      <c r="W2" s="46">
+        <v>1</v>
+      </c>
+      <c r="X2" s="46">
+        <v>1</v>
       </c>
       <c r="Y2" s="46" t="s">
         <v>64</v>
       </c>
-      <c r="Z2" s="46">
+      <c r="Z2" s="46" t="s">
+        <v>64</v>
+      </c>
+      <c r="AA2" s="46" t="s">
+        <v>64</v>
+      </c>
+      <c r="AB2" s="56">
         <v>1</v>
-      </c>
-      <c r="AA2" s="56">
-        <v>1</v>
-      </c>
-      <c r="AB2" s="46">
-        <v>10</v>
       </c>
       <c r="AC2" s="57">
         <v>44136</v>
@@ -2828,7 +2833,7 @@
         <v>2</v>
       </c>
       <c r="R3" s="46">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="S3" s="46">
         <v>2</v>
@@ -2842,23 +2847,23 @@
       <c r="V3" s="46">
         <v>2</v>
       </c>
-      <c r="W3" s="46" t="s">
-        <v>65</v>
-      </c>
-      <c r="X3" s="46" t="s">
-        <v>65</v>
+      <c r="W3" s="46">
+        <v>2</v>
+      </c>
+      <c r="X3" s="46">
+        <v>2</v>
       </c>
       <c r="Y3" s="46" t="s">
         <v>65</v>
       </c>
-      <c r="Z3" s="46">
+      <c r="Z3" s="46" t="s">
+        <v>65</v>
+      </c>
+      <c r="AA3" s="46" t="s">
+        <v>65</v>
+      </c>
+      <c r="AB3" s="56">
         <v>2</v>
-      </c>
-      <c r="AA3" s="56">
-        <v>2</v>
-      </c>
-      <c r="AB3" s="46">
-        <v>10</v>
       </c>
       <c r="AC3" s="57">
         <v>44137</v>
@@ -2917,7 +2922,7 @@
         <v>3</v>
       </c>
       <c r="R4" s="46">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="S4" s="46">
         <v>3</v>
@@ -2931,23 +2936,23 @@
       <c r="V4" s="46">
         <v>3</v>
       </c>
-      <c r="W4" s="46" t="s">
-        <v>66</v>
-      </c>
-      <c r="X4" s="46" t="s">
-        <v>66</v>
+      <c r="W4" s="46">
+        <v>3</v>
+      </c>
+      <c r="X4" s="46">
+        <v>3</v>
       </c>
       <c r="Y4" s="46" t="s">
         <v>66</v>
       </c>
-      <c r="Z4" s="46">
-        <v>3</v>
-      </c>
-      <c r="AA4" s="56">
+      <c r="Z4" s="46" t="s">
+        <v>66</v>
+      </c>
+      <c r="AA4" s="46" t="s">
+        <v>66</v>
+      </c>
+      <c r="AB4" s="56">
         <v>-3</v>
-      </c>
-      <c r="AB4" s="46">
-        <v>11</v>
       </c>
       <c r="AC4" s="57">
         <v>44138</v>
@@ -3006,7 +3011,7 @@
         <v>4</v>
       </c>
       <c r="R5" s="46">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="S5" s="46">
         <v>4</v>
@@ -3020,23 +3025,23 @@
       <c r="V5" s="46">
         <v>4</v>
       </c>
-      <c r="W5" s="46" t="s">
-        <v>67</v>
-      </c>
-      <c r="X5" s="46" t="s">
-        <v>67</v>
+      <c r="W5" s="46">
+        <v>4</v>
+      </c>
+      <c r="X5" s="46">
+        <v>4</v>
       </c>
       <c r="Y5" s="46" t="s">
         <v>67</v>
       </c>
-      <c r="Z5" s="46">
-        <v>4</v>
-      </c>
-      <c r="AA5" s="56">
+      <c r="Z5" s="46" t="s">
+        <v>67</v>
+      </c>
+      <c r="AA5" s="46" t="s">
+        <v>67</v>
+      </c>
+      <c r="AB5" s="56">
         <v>-4</v>
-      </c>
-      <c r="AB5" s="46">
-        <v>10</v>
       </c>
       <c r="AC5" s="57">
         <v>44139</v>
@@ -3092,10 +3097,10 @@
         <v>5</v>
       </c>
       <c r="Q6" s="46">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="R6" s="46">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="S6" s="46">
         <v>5</v>
@@ -3109,23 +3114,23 @@
       <c r="V6" s="46">
         <v>5</v>
       </c>
-      <c r="W6" s="46" t="s">
-        <v>68</v>
-      </c>
-      <c r="X6" s="46" t="s">
-        <v>68</v>
+      <c r="W6" s="46">
+        <v>5</v>
+      </c>
+      <c r="X6" s="46">
+        <v>5</v>
       </c>
       <c r="Y6" s="46" t="s">
         <v>68</v>
       </c>
-      <c r="Z6" s="46">
-        <v>10</v>
-      </c>
-      <c r="AA6" s="56">
+      <c r="Z6" s="46" t="s">
+        <v>68</v>
+      </c>
+      <c r="AA6" s="46" t="s">
+        <v>68</v>
+      </c>
+      <c r="AB6" s="56">
         <v>-5</v>
-      </c>
-      <c r="AB6" s="46">
-        <v>10</v>
       </c>
       <c r="AC6" s="57">
         <v>44140</v>
@@ -3184,7 +3189,7 @@
         <v>6</v>
       </c>
       <c r="R7" s="46">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="S7" s="46">
         <v>6</v>
@@ -3198,23 +3203,23 @@
       <c r="V7" s="46">
         <v>6</v>
       </c>
-      <c r="W7" s="46" t="s">
-        <v>69</v>
-      </c>
-      <c r="X7" s="46" t="s">
-        <v>69</v>
+      <c r="W7" s="46">
+        <v>6</v>
+      </c>
+      <c r="X7" s="46">
+        <v>6</v>
       </c>
       <c r="Y7" s="46" t="s">
         <v>69</v>
       </c>
-      <c r="Z7" s="46">
+      <c r="Z7" s="46" t="s">
+        <v>69</v>
+      </c>
+      <c r="AA7" s="46" t="s">
+        <v>69</v>
+      </c>
+      <c r="AB7" s="56">
         <v>6</v>
-      </c>
-      <c r="AA7" s="56">
-        <v>6</v>
-      </c>
-      <c r="AB7" s="46">
-        <v>20</v>
       </c>
       <c r="AC7" s="57">
         <v>44141</v>
@@ -3273,7 +3278,7 @@
         <v>7</v>
       </c>
       <c r="R8" s="46">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="S8" s="46">
         <v>7</v>
@@ -3287,23 +3292,23 @@
       <c r="V8" s="46">
         <v>7</v>
       </c>
-      <c r="W8" s="46" t="s">
-        <v>70</v>
-      </c>
-      <c r="X8" s="46" t="s">
-        <v>70</v>
+      <c r="W8" s="46">
+        <v>7</v>
+      </c>
+      <c r="X8" s="46">
+        <v>7</v>
       </c>
       <c r="Y8" s="46" t="s">
         <v>70</v>
       </c>
-      <c r="Z8" s="46">
+      <c r="Z8" s="46" t="s">
+        <v>70</v>
+      </c>
+      <c r="AA8" s="46" t="s">
+        <v>70</v>
+      </c>
+      <c r="AB8" s="56">
         <v>7</v>
-      </c>
-      <c r="AA8" s="56">
-        <v>7</v>
-      </c>
-      <c r="AB8" s="46">
-        <v>20</v>
       </c>
       <c r="AC8" s="57">
         <v>44142</v>
@@ -3359,10 +3364,11 @@
         <v>8</v>
       </c>
       <c r="Q9" s="46">
-        <v>8</v>
-      </c>
-      <c r="R9" s="46">
-        <v>8</v>
+        <v>10</v>
+      </c>
+      <c r="R9" s="46" t="str">
+        <f>"9"</f>
+        <v>9</v>
       </c>
       <c r="S9" s="46">
         <v>8</v>
@@ -3376,23 +3382,23 @@
       <c r="V9" s="46">
         <v>8</v>
       </c>
-      <c r="W9" s="46" t="s">
-        <v>71</v>
-      </c>
-      <c r="X9" s="46" t="s">
-        <v>71</v>
+      <c r="W9" s="46">
+        <v>8</v>
+      </c>
+      <c r="X9" s="46">
+        <v>8</v>
       </c>
       <c r="Y9" s="46" t="s">
         <v>71</v>
       </c>
-      <c r="Z9" s="46">
-        <v>10</v>
-      </c>
-      <c r="AA9" s="56">
+      <c r="Z9" s="46" t="s">
+        <v>71</v>
+      </c>
+      <c r="AA9" s="46" t="s">
+        <v>71</v>
+      </c>
+      <c r="AB9" s="56">
         <v>8</v>
-      </c>
-      <c r="AB9" s="46">
-        <v>10</v>
       </c>
       <c r="AC9" s="57">
         <v>44143</v>
@@ -3451,7 +3457,7 @@
         <v>9</v>
       </c>
       <c r="R10" s="46">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="S10" s="46">
         <v>9</v>
@@ -3465,23 +3471,23 @@
       <c r="V10" s="46">
         <v>9</v>
       </c>
-      <c r="W10" s="46" t="s">
-        <v>72</v>
-      </c>
-      <c r="X10" s="46" t="s">
-        <v>72</v>
+      <c r="W10" s="46">
+        <v>9</v>
+      </c>
+      <c r="X10" s="46">
+        <v>9</v>
       </c>
       <c r="Y10" s="46" t="s">
         <v>72</v>
       </c>
-      <c r="Z10" s="46">
+      <c r="Z10" s="46" t="s">
+        <v>72</v>
+      </c>
+      <c r="AA10" s="46" t="s">
+        <v>72</v>
+      </c>
+      <c r="AB10" s="56">
         <v>9</v>
-      </c>
-      <c r="AA10" s="56">
-        <v>9</v>
-      </c>
-      <c r="AB10" s="46">
-        <v>10</v>
       </c>
       <c r="AC10" s="57">
         <v>44144</v>
@@ -3536,7 +3542,8 @@
       <c r="P11" s="46">
         <v>10</v>
       </c>
-      <c r="Q11" s="46">
+      <c r="Q11" s="60" t="str">
+        <f>"10"</f>
         <v>10</v>
       </c>
       <c r="R11" s="46">
@@ -3554,30 +3561,30 @@
       <c r="V11" s="46">
         <v>10</v>
       </c>
-      <c r="W11" s="46" t="s">
-        <v>73</v>
-      </c>
-      <c r="X11" s="46" t="s">
-        <v>73</v>
+      <c r="W11" s="46">
+        <v>10</v>
+      </c>
+      <c r="X11" s="46">
+        <v>10</v>
       </c>
       <c r="Y11" s="46" t="s">
         <v>73</v>
       </c>
-      <c r="Z11" s="46">
-        <v>10</v>
-      </c>
-      <c r="AA11" s="56">
-        <v>10</v>
-      </c>
-      <c r="AB11" s="46">
+      <c r="Z11" s="46" t="s">
+        <v>73</v>
+      </c>
+      <c r="AA11" s="46" t="s">
+        <v>73</v>
+      </c>
+      <c r="AB11" s="56">
         <v>10</v>
       </c>
       <c r="AC11" s="57">
         <v>44145</v>
       </c>
     </row>
-    <row r="21" spans="19:19">
-      <c r="S21" t="s">
+    <row r="21" spans="21:21">
+      <c r="U21" t="s">
         <v>81</v>
       </c>
     </row>
@@ -3681,19 +3688,19 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I2:I11">
-    <cfRule type="top10" dxfId="35" priority="21" percent="1" rank="20"/>
+    <cfRule type="top10" dxfId="17" priority="21" percent="1" rank="20"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="J2:J11">
-    <cfRule type="top10" dxfId="34" priority="20" rank="5"/>
+    <cfRule type="top10" dxfId="16" priority="20" rank="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="K2:K11">
-    <cfRule type="top10" dxfId="33" priority="19" bottom="1" rank="5"/>
+    <cfRule type="top10" dxfId="15" priority="19" bottom="1" rank="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L2:L11">
-    <cfRule type="aboveAverage" dxfId="32" priority="18"/>
+    <cfRule type="aboveAverage" dxfId="14" priority="18"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="M2:M11">
-    <cfRule type="aboveAverage" dxfId="31" priority="17" aboveAverage="0"/>
+    <cfRule type="aboveAverage" dxfId="13" priority="17" aboveAverage="0"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="N2:N11">
     <cfRule type="iconSet" priority="16">
@@ -3724,65 +3731,65 @@
       </iconSet>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Q2:Q11">
-    <cfRule type="cellIs" dxfId="30" priority="13" operator="greaterThan">
+  <conditionalFormatting sqref="S2:S11">
+    <cfRule type="cellIs" dxfId="12" priority="13" operator="greaterThan">
       <formula>5.5</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S2:S11">
-    <cfRule type="cellIs" dxfId="29" priority="12" stopIfTrue="1" operator="equal">
+  <conditionalFormatting sqref="U2:U11">
+    <cfRule type="cellIs" dxfId="11" priority="12" stopIfTrue="1" operator="equal">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="R2:R11">
-    <cfRule type="cellIs" dxfId="28" priority="11" operator="lessThan">
+  <conditionalFormatting sqref="T2:T11">
+    <cfRule type="cellIs" dxfId="10" priority="11" operator="lessThan">
       <formula>5.5</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="T2:T11">
-    <cfRule type="cellIs" dxfId="27" priority="10" operator="notEqual">
+  <conditionalFormatting sqref="V2:V11">
+    <cfRule type="cellIs" dxfId="9" priority="10" operator="notEqual">
       <formula>5</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="U2:U11">
-    <cfRule type="cellIs" dxfId="26" priority="9" operator="greaterThanOrEqual">
+  <conditionalFormatting sqref="W2:W11">
+    <cfRule type="cellIs" dxfId="8" priority="9" operator="greaterThanOrEqual">
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="V2:V11">
-    <cfRule type="cellIs" dxfId="25" priority="8" operator="between">
+  <conditionalFormatting sqref="X2:X11">
+    <cfRule type="cellIs" dxfId="7" priority="8" operator="between">
       <formula>3</formula>
       <formula>8</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="W2:W11">
-    <cfRule type="containsText" dxfId="24" priority="7" operator="containsText" text="land">
-      <formula>NOT(ISERROR(SEARCH("land",W2)))</formula>
+  <conditionalFormatting sqref="Y2:Y11">
+    <cfRule type="containsText" dxfId="6" priority="7" operator="containsText" text="land">
+      <formula>NOT(ISERROR(SEARCH("land",Y2)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Y2:Y11">
-    <cfRule type="beginsWith" dxfId="23" priority="6" operator="beginsWith" text="S">
-      <formula>LEFT(Y2,1)="S"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="X2:X11">
-    <cfRule type="endsWith" dxfId="22" priority="5" operator="endsWith" text="ia">
-      <formula>RIGHT(X2,2)="ia"</formula>
+  <conditionalFormatting sqref="AA2:AA11">
+    <cfRule type="beginsWith" dxfId="5" priority="6" operator="beginsWith" text="S">
+      <formula>LEFT(AA2,1)="S"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z2:Z11">
-    <cfRule type="duplicateValues" dxfId="21" priority="4"/>
+    <cfRule type="endsWith" dxfId="4" priority="5" operator="endsWith" text="ia">
+      <formula>RIGHT(Z2,2)="ia"</formula>
+    </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AA2:AA11">
-    <cfRule type="cellIs" dxfId="20" priority="3" operator="lessThan">
+  <conditionalFormatting sqref="Q2:Q11">
+    <cfRule type="duplicateValues" dxfId="3" priority="4"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AB2:AB11">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AB2:AB11">
-    <cfRule type="uniqueValues" dxfId="19" priority="2"/>
+  <conditionalFormatting sqref="R2:R11">
+    <cfRule type="uniqueValues" dxfId="1" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="AC2:AC11">
-    <cfRule type="timePeriod" dxfId="18" priority="1" timePeriod="lastWeek">
+    <cfRule type="timePeriod" dxfId="0" priority="1" timePeriod="lastWeek">
       <formula>AND(TODAY()-ROUNDDOWN(AC2,0)&gt;=(WEEKDAY(TODAY())),TODAY()-ROUNDDOWN(AC2,0)&lt;(WEEKDAY(TODAY())+7))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Implemented operator based conditional styling (issue #5).
</commit_message>
<xml_diff>
--- a/backend/test/assets/sample.xlsx
+++ b/backend/test/assets/sample.xlsx
@@ -397,9 +397,9 @@
     <numFmt numFmtId="164" formatCode="[$$-409]#,##0.0;[Red]\-[$$-409]#,##0.0"/>
     <numFmt numFmtId="165" formatCode="#,##0.00\ [$PLN];[Red]\-#,##0.00\ [$PLN]"/>
     <numFmt numFmtId="166" formatCode="mm/dd/yy;@"/>
-    <numFmt numFmtId="168" formatCode="0.00_);[Red]\(0.00\)"/>
-    <numFmt numFmtId="169" formatCode="&quot;$&quot;#,##0.00"/>
-    <numFmt numFmtId="171" formatCode="\T\o\p\ @"/>
+    <numFmt numFmtId="167" formatCode="0.00_);[Red]\(0.00\)"/>
+    <numFmt numFmtId="168" formatCode="&quot;$&quot;#,##0.00"/>
+    <numFmt numFmtId="169" formatCode="\T\o\p\ @"/>
   </numFmts>
   <fonts count="9">
     <font>
@@ -858,13 +858,10 @@
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
     <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -876,14 +873,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="72">
+  <dxfs count="36">
     <dxf>
       <font>
         <condense val="0"/>
@@ -912,7 +912,7 @@
       <font>
         <color rgb="FFFFFF00"/>
       </font>
-      <numFmt numFmtId="168" formatCode="0.00_);[Red]\(0.00\)"/>
+      <numFmt numFmtId="167" formatCode="0.00_);[Red]\(0.00\)"/>
       <fill>
         <patternFill>
           <bgColor rgb="FF00B050"/>
@@ -1130,9 +1130,21 @@
     </dxf>
     <dxf>
       <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FFFFFF00"/>
       </font>
-      <numFmt numFmtId="168" formatCode="0.00_);[Red]\(0.00\)"/>
+      <numFmt numFmtId="167" formatCode="0.00_);[Red]\(0.00\)"/>
       <fill>
         <patternFill>
           <bgColor rgb="FF00B050"/>
@@ -1155,460 +1167,6 @@
       <fill>
         <patternFill>
           <bgColor theme="5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFFFF00"/>
-      </font>
-      <numFmt numFmtId="14" formatCode="0.00%"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <numFmt numFmtId="14" formatCode="0.00%"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2422,10 +1980,10 @@
       </c>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3" s="54" t="s">
+      <c r="A3" s="60" t="s">
         <v>30</v>
       </c>
-      <c r="B3" s="54"/>
+      <c r="B3" s="60"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2580,8 +2138,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AC21"/>
   <sheetViews>
-    <sheetView topLeftCell="O1" workbookViewId="0">
-      <selection activeCell="Q13" sqref="Q13"/>
+    <sheetView topLeftCell="P1" workbookViewId="0">
+      <selection activeCell="AA2" sqref="AA2:AA11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2728,7 +2286,7 @@
       <c r="L2" s="46">
         <v>10</v>
       </c>
-      <c r="M2" s="55">
+      <c r="M2" s="54">
         <v>-10</v>
       </c>
       <c r="N2" s="46">
@@ -2773,10 +2331,10 @@
       <c r="AA2" s="46" t="s">
         <v>64</v>
       </c>
-      <c r="AB2" s="56">
+      <c r="AB2" s="55">
         <v>1</v>
       </c>
-      <c r="AC2" s="57">
+      <c r="AC2" s="56">
         <v>44136</v>
       </c>
     </row>
@@ -2817,7 +2375,7 @@
       <c r="L3" s="46">
         <v>20</v>
       </c>
-      <c r="M3" s="55">
+      <c r="M3" s="54">
         <v>20</v>
       </c>
       <c r="N3" s="46">
@@ -2862,10 +2420,10 @@
       <c r="AA3" s="46" t="s">
         <v>65</v>
       </c>
-      <c r="AB3" s="56">
+      <c r="AB3" s="55">
         <v>2</v>
       </c>
-      <c r="AC3" s="57">
+      <c r="AC3" s="56">
         <v>44137</v>
       </c>
     </row>
@@ -2906,7 +2464,7 @@
       <c r="L4" s="46">
         <v>30</v>
       </c>
-      <c r="M4" s="55">
+      <c r="M4" s="54">
         <v>30</v>
       </c>
       <c r="N4" s="46">
@@ -2951,10 +2509,10 @@
       <c r="AA4" s="46" t="s">
         <v>66</v>
       </c>
-      <c r="AB4" s="56">
+      <c r="AB4" s="55">
         <v>-3</v>
       </c>
-      <c r="AC4" s="57">
+      <c r="AC4" s="56">
         <v>44138</v>
       </c>
     </row>
@@ -2995,7 +2553,7 @@
       <c r="L5" s="46">
         <v>40</v>
       </c>
-      <c r="M5" s="55">
+      <c r="M5" s="54">
         <v>40</v>
       </c>
       <c r="N5" s="46">
@@ -3040,10 +2598,10 @@
       <c r="AA5" s="46" t="s">
         <v>67</v>
       </c>
-      <c r="AB5" s="56">
+      <c r="AB5" s="55">
         <v>-4</v>
       </c>
-      <c r="AC5" s="57">
+      <c r="AC5" s="56">
         <v>44139</v>
       </c>
     </row>
@@ -3084,7 +2642,7 @@
       <c r="L6" s="46">
         <v>50</v>
       </c>
-      <c r="M6" s="55">
+      <c r="M6" s="54">
         <v>50</v>
       </c>
       <c r="N6" s="46">
@@ -3129,10 +2687,10 @@
       <c r="AA6" s="46" t="s">
         <v>68</v>
       </c>
-      <c r="AB6" s="56">
+      <c r="AB6" s="55">
         <v>-5</v>
       </c>
-      <c r="AC6" s="57">
+      <c r="AC6" s="56">
         <v>44140</v>
       </c>
     </row>
@@ -3158,7 +2716,7 @@
       <c r="G7" s="46">
         <v>6</v>
       </c>
-      <c r="H7" s="58">
+      <c r="H7" s="57">
         <v>10</v>
       </c>
       <c r="I7" s="46">
@@ -3173,7 +2731,7 @@
       <c r="L7" s="46">
         <v>60</v>
       </c>
-      <c r="M7" s="55">
+      <c r="M7" s="54">
         <v>60</v>
       </c>
       <c r="N7" s="46">
@@ -3218,10 +2776,10 @@
       <c r="AA7" s="46" t="s">
         <v>69</v>
       </c>
-      <c r="AB7" s="56">
+      <c r="AB7" s="55">
         <v>6</v>
       </c>
-      <c r="AC7" s="57">
+      <c r="AC7" s="56">
         <v>44141</v>
       </c>
     </row>
@@ -3262,7 +2820,7 @@
       <c r="L8" s="46">
         <v>70</v>
       </c>
-      <c r="M8" s="55">
+      <c r="M8" s="54">
         <v>70</v>
       </c>
       <c r="N8" s="46">
@@ -3307,10 +2865,10 @@
       <c r="AA8" s="46" t="s">
         <v>70</v>
       </c>
-      <c r="AB8" s="56">
+      <c r="AB8" s="55">
         <v>7</v>
       </c>
-      <c r="AC8" s="57">
+      <c r="AC8" s="56">
         <v>44142</v>
       </c>
     </row>
@@ -3351,7 +2909,7 @@
       <c r="L9" s="46">
         <v>80</v>
       </c>
-      <c r="M9" s="55">
+      <c r="M9" s="54">
         <v>80</v>
       </c>
       <c r="N9" s="46">
@@ -3397,10 +2955,10 @@
       <c r="AA9" s="46" t="s">
         <v>71</v>
       </c>
-      <c r="AB9" s="56">
+      <c r="AB9" s="55">
         <v>8</v>
       </c>
-      <c r="AC9" s="57">
+      <c r="AC9" s="56">
         <v>44143</v>
       </c>
     </row>
@@ -3441,7 +2999,7 @@
       <c r="L10" s="46">
         <v>90</v>
       </c>
-      <c r="M10" s="55">
+      <c r="M10" s="54">
         <v>90</v>
       </c>
       <c r="N10" s="46">
@@ -3486,10 +3044,10 @@
       <c r="AA10" s="46" t="s">
         <v>72</v>
       </c>
-      <c r="AB10" s="56">
+      <c r="AB10" s="55">
         <v>9</v>
       </c>
-      <c r="AC10" s="57">
+      <c r="AC10" s="56">
         <v>44144</v>
       </c>
     </row>
@@ -3512,7 +3070,7 @@
       <c r="F11" s="51">
         <v>10</v>
       </c>
-      <c r="G11" s="59">
+      <c r="G11" s="58">
         <v>10</v>
       </c>
       <c r="H11" s="46">
@@ -3530,7 +3088,7 @@
       <c r="L11" s="46">
         <v>100</v>
       </c>
-      <c r="M11" s="55">
+      <c r="M11" s="54">
         <v>100</v>
       </c>
       <c r="N11" s="46">
@@ -3542,7 +3100,7 @@
       <c r="P11" s="46">
         <v>10</v>
       </c>
-      <c r="Q11" s="60" t="str">
+      <c r="Q11" s="59" t="str">
         <f>"10"</f>
         <v>10</v>
       </c>
@@ -3576,10 +3134,10 @@
       <c r="AA11" s="46" t="s">
         <v>73</v>
       </c>
-      <c r="AB11" s="56">
+      <c r="AB11" s="55">
         <v>10</v>
       </c>
-      <c r="AC11" s="57">
+      <c r="AC11" s="56">
         <v>44145</v>
       </c>
     </row>
@@ -3688,19 +3246,19 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I2:I11">
-    <cfRule type="top10" dxfId="17" priority="21" percent="1" rank="20"/>
+    <cfRule type="top10" dxfId="35" priority="21" percent="1" rank="20"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="J2:J11">
-    <cfRule type="top10" dxfId="16" priority="20" rank="5"/>
+    <cfRule type="top10" dxfId="34" priority="20" rank="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="K2:K11">
-    <cfRule type="top10" dxfId="15" priority="19" bottom="1" rank="5"/>
+    <cfRule type="top10" dxfId="33" priority="19" bottom="1" rank="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L2:L11">
-    <cfRule type="aboveAverage" dxfId="14" priority="18"/>
+    <cfRule type="aboveAverage" dxfId="32" priority="18"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="M2:M11">
-    <cfRule type="aboveAverage" dxfId="13" priority="17" aboveAverage="0"/>
+    <cfRule type="aboveAverage" dxfId="31" priority="17" aboveAverage="0"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="N2:N11">
     <cfRule type="iconSet" priority="16">
@@ -3732,64 +3290,64 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S2:S11">
-    <cfRule type="cellIs" dxfId="12" priority="13" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="30" priority="13" operator="greaterThan">
       <formula>5.5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U2:U11">
-    <cfRule type="cellIs" dxfId="11" priority="12" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="12" stopIfTrue="1" operator="equal">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T2:T11">
-    <cfRule type="cellIs" dxfId="10" priority="11" operator="lessThan">
+    <cfRule type="cellIs" dxfId="28" priority="11" operator="lessThan">
       <formula>5.5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V2:V11">
-    <cfRule type="cellIs" dxfId="9" priority="10" operator="notEqual">
+    <cfRule type="cellIs" dxfId="27" priority="10" operator="notEqual">
       <formula>5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W2:W11">
-    <cfRule type="cellIs" dxfId="8" priority="9" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="26" priority="9" operator="greaterThanOrEqual">
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X2:X11">
-    <cfRule type="cellIs" dxfId="7" priority="8" operator="between">
+    <cfRule type="cellIs" dxfId="25" priority="8" operator="between">
       <formula>3</formula>
       <formula>8</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y2:Y11">
-    <cfRule type="containsText" dxfId="6" priority="7" operator="containsText" text="land">
+    <cfRule type="containsText" dxfId="24" priority="7" operator="containsText" text="land">
       <formula>NOT(ISERROR(SEARCH("land",Y2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA2:AA11">
-    <cfRule type="beginsWith" dxfId="5" priority="6" operator="beginsWith" text="S">
-      <formula>LEFT(AA2,1)="S"</formula>
+    <cfRule type="beginsWith" dxfId="18" priority="6" operator="beginsWith" text="s">
+      <formula>LEFT(AA2,1)="s"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z2:Z11">
-    <cfRule type="endsWith" dxfId="4" priority="5" operator="endsWith" text="ia">
+    <cfRule type="endsWith" dxfId="23" priority="5" operator="endsWith" text="ia">
       <formula>RIGHT(Z2,2)="ia"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q2:Q11">
-    <cfRule type="duplicateValues" dxfId="3" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="22" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB2:AB11">
-    <cfRule type="cellIs" dxfId="2" priority="3" operator="lessThan">
+    <cfRule type="cellIs" dxfId="21" priority="3" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R2:R11">
-    <cfRule type="uniqueValues" dxfId="1" priority="2"/>
+    <cfRule type="uniqueValues" dxfId="20" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="AC2:AC11">
-    <cfRule type="timePeriod" dxfId="0" priority="1" timePeriod="lastWeek">
+    <cfRule type="timePeriod" dxfId="19" priority="1" timePeriod="lastWeek">
       <formula>AND(TODAY()-ROUNDDOWN(AC2,0)&gt;=(WEEKDAY(TODAY())),TODAY()-ROUNDDOWN(AC2,0)&lt;(WEEKDAY(TODAY())+7))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Added CSV parsing (issue #2). Simplified Excel meta data handling.
</commit_message>
<xml_diff>
--- a/backend/test/assets/sample.xlsx
+++ b/backend/test/assets/sample.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500"/>
+    <workbookView xWindow="15" yWindow="1560" windowWidth="16380" windowHeight="8190" tabRatio="500" firstSheet="1" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Text (with styles)" sheetId="1" r:id="rId1"/>
@@ -1056,7 +1056,89 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="18">
+  <dxfs count="24">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1605,7 +1687,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A39" sqref="A39"/>
     </sheetView>
   </sheetViews>
@@ -2088,8 +2170,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AC21"/>
   <sheetViews>
-    <sheetView topLeftCell="P1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AA2" sqref="AA2"/>
+    <sheetView tabSelected="1" topLeftCell="N1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Y2" sqref="Y2:AA11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2101,18 +2183,23 @@
     <col min="5" max="5" width="4" customWidth="1"/>
     <col min="6" max="6" width="8.28515625" customWidth="1"/>
     <col min="7" max="7" width="9.7109375" customWidth="1"/>
-    <col min="8" max="11" width="8.5703125" customWidth="1"/>
+    <col min="8" max="8" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="10.140625" customWidth="1"/>
-    <col min="13" max="13" width="10.28515625" customWidth="1"/>
-    <col min="14" max="16" width="8.5703125" customWidth="1"/>
-    <col min="17" max="17" width="15.140625" customWidth="1"/>
-    <col min="18" max="18" width="8.5703125" customWidth="1"/>
+    <col min="13" max="13" width="10" bestFit="1" customWidth="1"/>
+    <col min="14" max="16" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="7.42578125" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="12.140625" customWidth="1"/>
-    <col min="20" max="22" width="8.5703125" customWidth="1"/>
+    <col min="20" max="20" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="15.5703125" customWidth="1"/>
-    <col min="24" max="24" width="8.5703125" customWidth="1"/>
+    <col min="24" max="24" width="9" bestFit="1" customWidth="1"/>
     <col min="25" max="27" width="14.42578125" customWidth="1"/>
-    <col min="28" max="28" width="8.5703125" customWidth="1"/>
+    <col min="28" max="28" width="7.28515625" bestFit="1" customWidth="1"/>
     <col min="29" max="29" width="10.7109375" customWidth="1"/>
     <col min="30" max="1025" width="8.5703125" customWidth="1"/>
   </cols>
@@ -2279,13 +2366,13 @@
       <c r="X2" s="30">
         <v>1</v>
       </c>
-      <c r="Y2" s="2" t="s">
+      <c r="Y2" s="30" t="s">
         <v>79</v>
       </c>
-      <c r="Z2" s="2" t="s">
+      <c r="Z2" s="30" t="s">
         <v>79</v>
       </c>
-      <c r="AA2" s="2" t="s">
+      <c r="AA2" s="30" t="s">
         <v>79</v>
       </c>
       <c r="AB2" s="32">
@@ -2368,13 +2455,13 @@
       <c r="X3" s="30">
         <v>2</v>
       </c>
-      <c r="Y3" s="2" t="s">
+      <c r="Y3" s="30" t="s">
         <v>80</v>
       </c>
-      <c r="Z3" s="2" t="s">
+      <c r="Z3" s="30" t="s">
         <v>80</v>
       </c>
-      <c r="AA3" s="2" t="s">
+      <c r="AA3" s="30" t="s">
         <v>80</v>
       </c>
       <c r="AB3" s="32">
@@ -2457,13 +2544,13 @@
       <c r="X4" s="30">
         <v>3</v>
       </c>
-      <c r="Y4" s="2" t="s">
+      <c r="Y4" s="30" t="s">
         <v>81</v>
       </c>
-      <c r="Z4" s="2" t="s">
+      <c r="Z4" s="30" t="s">
         <v>81</v>
       </c>
-      <c r="AA4" s="2" t="s">
+      <c r="AA4" s="30" t="s">
         <v>81</v>
       </c>
       <c r="AB4" s="32">
@@ -2546,13 +2633,13 @@
       <c r="X5" s="30">
         <v>4</v>
       </c>
-      <c r="Y5" s="2" t="s">
+      <c r="Y5" s="30" t="s">
         <v>82</v>
       </c>
-      <c r="Z5" s="2" t="s">
+      <c r="Z5" s="30" t="s">
         <v>82</v>
       </c>
-      <c r="AA5" s="2" t="s">
+      <c r="AA5" s="30" t="s">
         <v>82</v>
       </c>
       <c r="AB5" s="32">
@@ -2635,13 +2722,13 @@
       <c r="X6" s="30">
         <v>5</v>
       </c>
-      <c r="Y6" s="2" t="s">
+      <c r="Y6" s="30" t="s">
         <v>83</v>
       </c>
-      <c r="Z6" s="2" t="s">
+      <c r="Z6" s="30" t="s">
         <v>83</v>
       </c>
-      <c r="AA6" s="2" t="s">
+      <c r="AA6" s="30" t="s">
         <v>83</v>
       </c>
       <c r="AB6" s="32">
@@ -2724,13 +2811,13 @@
       <c r="X7" s="30">
         <v>6</v>
       </c>
-      <c r="Y7" s="2" t="s">
+      <c r="Y7" s="30" t="s">
         <v>84</v>
       </c>
-      <c r="Z7" s="2" t="s">
+      <c r="Z7" s="30" t="s">
         <v>84</v>
       </c>
-      <c r="AA7" s="2" t="s">
+      <c r="AA7" s="30" t="s">
         <v>84</v>
       </c>
       <c r="AB7" s="32">
@@ -2813,13 +2900,13 @@
       <c r="X8" s="30">
         <v>7</v>
       </c>
-      <c r="Y8" s="2" t="s">
+      <c r="Y8" s="30" t="s">
         <v>85</v>
       </c>
-      <c r="Z8" s="2" t="s">
+      <c r="Z8" s="30" t="s">
         <v>85</v>
       </c>
-      <c r="AA8" s="2" t="s">
+      <c r="AA8" s="30" t="s">
         <v>85</v>
       </c>
       <c r="AB8" s="32">
@@ -2903,13 +2990,13 @@
       <c r="X9" s="30">
         <v>8</v>
       </c>
-      <c r="Y9" s="2" t="s">
+      <c r="Y9" s="30" t="s">
         <v>86</v>
       </c>
-      <c r="Z9" s="2" t="s">
+      <c r="Z9" s="30" t="s">
         <v>86</v>
       </c>
-      <c r="AA9" s="2" t="s">
+      <c r="AA9" s="30" t="s">
         <v>86</v>
       </c>
       <c r="AB9" s="32">
@@ -2992,13 +3079,13 @@
       <c r="X10" s="30">
         <v>9</v>
       </c>
-      <c r="Y10" s="2" t="s">
+      <c r="Y10" s="30" t="s">
         <v>87</v>
       </c>
-      <c r="Z10" s="2" t="s">
+      <c r="Z10" s="30" t="s">
         <v>87</v>
       </c>
-      <c r="AA10" s="2" t="s">
+      <c r="AA10" s="30" t="s">
         <v>87</v>
       </c>
       <c r="AB10" s="32">
@@ -3082,13 +3169,13 @@
       <c r="X11" s="30">
         <v>10</v>
       </c>
-      <c r="Y11" s="2" t="s">
+      <c r="Y11" s="30" t="s">
         <v>88</v>
       </c>
-      <c r="Z11" s="2" t="s">
+      <c r="Z11" s="30" t="s">
         <v>88</v>
       </c>
-      <c r="AA11" s="2" t="s">
+      <c r="AA11" s="30" t="s">
         <v>88</v>
       </c>
       <c r="AB11" s="32">
@@ -3105,7 +3192,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:A11">
-    <cfRule type="colorScale" priority="2">
+    <cfRule type="colorScale" priority="6">
       <colorScale>
         <cfvo type="num" val="1"/>
         <cfvo type="num" val="100"/>
@@ -3113,7 +3200,7 @@
         <color rgb="FFFFEF9C"/>
       </colorScale>
     </cfRule>
-    <cfRule type="colorScale" priority="3">
+    <cfRule type="colorScale" priority="7">
       <colorScale>
         <cfvo type="min" val="0"/>
         <cfvo type="percentile" val="50"/>
@@ -3125,7 +3212,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:B11">
-    <cfRule type="colorScale" priority="4">
+    <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="percentile" val="10"/>
         <cfvo type="percentile" val="50"/>
@@ -3137,7 +3224,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2:C11">
-    <cfRule type="colorScale" priority="5">
+    <cfRule type="colorScale" priority="9">
       <colorScale>
         <cfvo type="percent" val="0"/>
         <cfvo type="percent" val="50"/>
@@ -3149,7 +3236,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2:D11">
-    <cfRule type="colorScale" priority="6">
+    <cfRule type="colorScale" priority="10">
       <colorScale>
         <cfvo type="min" val="0"/>
         <cfvo type="percent" val="50"/>
@@ -3161,7 +3248,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:E11">
-    <cfRule type="colorScale" priority="7">
+    <cfRule type="colorScale" priority="11">
       <colorScale>
         <cfvo type="formula" val="$B$2"/>
         <cfvo type="formula" val="$B$6"/>
@@ -3173,7 +3260,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2:F11">
-    <cfRule type="colorScale" priority="8">
+    <cfRule type="colorScale" priority="12">
       <colorScale>
         <cfvo type="formula" val="$B$2"/>
         <cfvo type="formula" val="$B$6*4"/>
@@ -3185,7 +3272,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G2:G11">
-    <cfRule type="dataBar" priority="9">
+    <cfRule type="dataBar" priority="13">
       <dataBar>
         <cfvo type="min" val="0"/>
         <cfvo type="max" val="0"/>
@@ -3199,7 +3286,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2:H11">
-    <cfRule type="dataBar" priority="10">
+    <cfRule type="dataBar" priority="14">
       <dataBar showValue="0">
         <cfvo type="min" val="0"/>
         <cfvo type="max" val="0"/>
@@ -3213,22 +3300,22 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I2:I11">
-    <cfRule type="top10" dxfId="17" priority="11" percent="1" rank="20"/>
+    <cfRule type="top10" dxfId="23" priority="15" percent="1" rank="20"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="J2:J11">
-    <cfRule type="top10" dxfId="16" priority="12" rank="5"/>
+    <cfRule type="top10" dxfId="22" priority="16" rank="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="K2:K11">
-    <cfRule type="top10" dxfId="15" priority="13" bottom="1" rank="5"/>
+    <cfRule type="top10" dxfId="21" priority="17" bottom="1" rank="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L2:L11">
-    <cfRule type="aboveAverage" dxfId="14" priority="14"/>
+    <cfRule type="aboveAverage" dxfId="20" priority="18"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="M2:M11">
-    <cfRule type="aboveAverage" dxfId="13" priority="15" aboveAverage="0"/>
+    <cfRule type="aboveAverage" dxfId="19" priority="19" aboveAverage="0"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="N2:N11">
-    <cfRule type="iconSet" priority="16">
+    <cfRule type="iconSet" priority="20">
       <iconSet iconSet="3Flags" reverse="1">
         <cfvo type="percent" val="0"/>
         <cfvo type="num" val="4"/>
@@ -3237,7 +3324,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O2:O11">
-    <cfRule type="iconSet" priority="17">
+    <cfRule type="iconSet" priority="21">
       <iconSet iconSet="5ArrowsGray">
         <cfvo type="percent" val="0"/>
         <cfvo type="percent" val="20"/>
@@ -3248,7 +3335,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P2:P11">
-    <cfRule type="iconSet" priority="18">
+    <cfRule type="iconSet" priority="22">
       <iconSet iconSet="3Symbols2" showValue="0">
         <cfvo type="percent" val="0"/>
         <cfvo type="percent" val="33"/>
@@ -3257,59 +3344,83 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S2:S11">
-    <cfRule type="cellIs" dxfId="12" priority="19" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="18" priority="23" operator="greaterThan">
       <formula>5.5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U2:U11">
-    <cfRule type="cellIs" dxfId="11" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="24" operator="equal">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T2:T11">
-    <cfRule type="cellIs" dxfId="10" priority="21" operator="lessThan">
+    <cfRule type="cellIs" dxfId="16" priority="25" operator="lessThan">
       <formula>5.5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V2:V11">
-    <cfRule type="cellIs" dxfId="9" priority="22" operator="notEqual">
+    <cfRule type="cellIs" dxfId="15" priority="26" operator="notEqual">
       <formula>5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W2:W11">
-    <cfRule type="cellIs" dxfId="8" priority="23" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="14" priority="27" operator="greaterThanOrEqual">
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X2:X11">
-    <cfRule type="cellIs" dxfId="7" priority="24" operator="between">
+    <cfRule type="cellIs" dxfId="13" priority="28" operator="between">
       <formula>3</formula>
       <formula>8</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y2:Y11">
-    <cfRule type="containsText" dxfId="6" priority="25" operator="containsText" text="land"/>
+    <cfRule type="containsText" dxfId="12" priority="29" operator="containsText" text="land"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA2:AA11">
-    <cfRule type="beginsWith" dxfId="5" priority="26" operator="beginsWith" text="s"/>
+    <cfRule type="beginsWith" dxfId="11" priority="30" operator="beginsWith" text="s"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z2:Z11">
-    <cfRule type="endsWith" dxfId="4" priority="27" operator="endsWith" text="ia"/>
+    <cfRule type="endsWith" dxfId="10" priority="31" operator="endsWith" text="ia"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q2:Q11">
-    <cfRule type="duplicateValues" dxfId="3" priority="28"/>
+    <cfRule type="duplicateValues" dxfId="9" priority="32"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB2:AB11">
-    <cfRule type="cellIs" dxfId="2" priority="29" operator="lessThan">
+    <cfRule type="cellIs" dxfId="8" priority="33" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R2:R11">
-    <cfRule type="uniqueValues" dxfId="1" priority="30"/>
+    <cfRule type="uniqueValues" dxfId="7" priority="34"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="AC2:AC11">
-    <cfRule type="timePeriod" dxfId="0" priority="31" timePeriod="lastWeek">
+    <cfRule type="timePeriod" dxfId="6" priority="35" timePeriod="lastWeek">
       <formula>AND(TODAY()-ROUNDDOWN(AC2,0)&gt;=(WEEKDAY(TODAY())),TODAY()-ROUNDDOWN(AC2,0)&lt;(WEEKDAY(TODAY())+7))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N2:N11">
+    <cfRule type="iconSet" priority="4">
+      <iconSet iconSet="3Flags" reverse="1">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="num" val="4" gte="0"/>
+        <cfvo type="num" val="8"/>
+      </iconSet>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Y2:Y11">
+    <cfRule type="containsText" dxfId="5" priority="3" operator="containsText" text="land">
+      <formula>NOT(ISERROR(SEARCH("land",Y2)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AA2:AA11">
+    <cfRule type="beginsWith" dxfId="3" priority="2" operator="beginsWith" text="s">
+      <formula>LEFT(AA2,1)="s"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Z2:Z11">
+    <cfRule type="endsWith" dxfId="1" priority="1" operator="endsWith" text="ia">
+      <formula>RIGHT(Z2,2)="ia"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>

</xml_diff>